<commit_message>
alterado nome do ctap
</commit_message>
<xml_diff>
--- a/relatorio_iteracoes_NR.xlsx
+++ b/relatorio_iteracoes_NR.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -564,7 +564,7 @@
         <v>1.045</v>
       </c>
       <c r="L3" t="n">
-        <v>-4.73314</v>
+        <v>-4.74283</v>
       </c>
     </row>
     <row r="4">
@@ -600,7 +600,7 @@
         <v>1.01</v>
       </c>
       <c r="L4" t="n">
-        <v>-12.32479</v>
+        <v>-12.34593</v>
       </c>
     </row>
     <row r="5">
@@ -633,10 +633,10 @@
       </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="n">
-        <v>1.02428</v>
+        <v>1.01042</v>
       </c>
       <c r="L5" t="n">
-        <v>-10.07866</v>
+        <v>-9.80561</v>
       </c>
     </row>
     <row r="6">
@@ -669,10 +669,10 @@
       </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="n">
-        <v>1.02619</v>
+        <v>1.01936</v>
       </c>
       <c r="L6" t="n">
-        <v>-8.55809</v>
+        <v>-8.48696</v>
       </c>
     </row>
     <row r="7">
@@ -695,20 +695,20 @@
         <v>-0.112</v>
       </c>
       <c r="G7" t="n">
-        <v>0.047</v>
+        <v>0.165</v>
       </c>
       <c r="H7" t="n">
         <v>-0.20551</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>-0.03687</v>
       </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="n">
-        <v>1.07</v>
+        <v>1.08848</v>
       </c>
       <c r="L7" t="n">
-        <v>-13.95243</v>
+        <v>-14.31205</v>
       </c>
     </row>
     <row r="8">
@@ -741,10 +741,10 @@
       </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="n">
-        <v>1.07206</v>
+        <v>1</v>
       </c>
       <c r="L8" t="n">
-        <v>-13.23205</v>
+        <v>-12.72817</v>
       </c>
     </row>
     <row r="9">
@@ -767,20 +767,20 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.174</v>
+        <v>-0.06</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>-0.38291</v>
       </c>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="n">
-        <v>1.09</v>
+        <v>0.93876</v>
       </c>
       <c r="L9" t="n">
-        <v>-13.23205</v>
+        <v>-12.72817</v>
       </c>
     </row>
     <row r="10">
@@ -813,10 +813,10 @@
       </c>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="n">
-        <v>1.06419</v>
+        <v>1.02081</v>
       </c>
       <c r="L10" t="n">
-        <v>-14.86881</v>
+        <v>-14.24512</v>
       </c>
     </row>
     <row r="11">
@@ -849,10 +849,10 @@
       </c>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="n">
-        <v>1.05784</v>
+        <v>1.02516</v>
       </c>
       <c r="L11" t="n">
-        <v>-14.99687</v>
+        <v>-14.51409</v>
       </c>
     </row>
     <row r="12">
@@ -885,10 +885,10 @@
       </c>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="n">
-        <v>1.06044</v>
+        <v>1.05279</v>
       </c>
       <c r="L12" t="n">
-        <v>-14.61146</v>
+        <v>-14.51353</v>
       </c>
     </row>
     <row r="13">
@@ -921,10 +921,10 @@
       </c>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="n">
-        <v>1.05624</v>
+        <v>1.07</v>
       </c>
       <c r="L13" t="n">
-        <v>-14.80784</v>
+        <v>-15.13733</v>
       </c>
     </row>
     <row r="14">
@@ -957,10 +957,10 @@
       </c>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="n">
-        <v>1.05185</v>
+        <v>1.06151</v>
       </c>
       <c r="L14" t="n">
-        <v>-14.91565</v>
+        <v>-15.11322</v>
       </c>
     </row>
     <row r="15">
@@ -993,10 +993,10 @@
       </c>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="n">
-        <v>1.04108</v>
+        <v>1.0205</v>
       </c>
       <c r="L15" t="n">
-        <v>-15.89096</v>
+        <v>-15.61139</v>
       </c>
     </row>
     <row r="16">
@@ -1007,13 +1007,13 @@
         <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>0.10664</v>
+        <v>0.26638</v>
       </c>
       <c r="D16" t="n">
-        <v>2.22816</v>
+        <v>2.22805</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.17688</v>
+        <v>-0.14566</v>
       </c>
       <c r="F16" t="n">
         <v>2.324</v>
@@ -1043,13 +1043,13 @@
         <v>2</v>
       </c>
       <c r="C17" t="n">
-        <v>0.10664</v>
+        <v>0.26638</v>
       </c>
       <c r="D17" t="n">
-        <v>0.22779</v>
+        <v>0.21778</v>
       </c>
       <c r="E17" t="n">
-        <v>0.20529</v>
+        <v>0.32852</v>
       </c>
       <c r="F17" t="n">
         <v>0.183</v>
@@ -1058,7 +1058,7 @@
         <v>0.12014</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.04479</v>
+        <v>-0.03478</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -1068,7 +1068,7 @@
         <v>1.045</v>
       </c>
       <c r="L17" t="n">
-        <v>-4.98098</v>
+        <v>-4.98487</v>
       </c>
     </row>
     <row r="18">
@@ -1079,13 +1079,13 @@
         <v>3</v>
       </c>
       <c r="C18" t="n">
-        <v>0.10664</v>
+        <v>0.26638</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.92897</v>
+        <v>-0.92549</v>
       </c>
       <c r="E18" t="n">
-        <v>0.01604</v>
+        <v>0.09772</v>
       </c>
       <c r="F18" t="n">
         <v>-0.9419999999999999</v>
@@ -1094,7 +1094,7 @@
         <v>-0.24398</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.01303</v>
+        <v>-0.01651</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
@@ -1104,7 +1104,7 @@
         <v>1.01</v>
       </c>
       <c r="L18" t="n">
-        <v>-12.7219</v>
+        <v>-12.74759</v>
       </c>
     </row>
     <row r="19">
@@ -1115,13 +1115,13 @@
         <v>4</v>
       </c>
       <c r="C19" t="n">
-        <v>0.10664</v>
+        <v>0.26638</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.4504</v>
+        <v>-0.46791</v>
       </c>
       <c r="E19" t="n">
-        <v>0.09079</v>
+        <v>0.08314000000000001</v>
       </c>
       <c r="F19" t="n">
         <v>-0.478</v>
@@ -1130,17 +1130,17 @@
         <v>0.039</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.0276</v>
+        <v>-0.01009</v>
       </c>
       <c r="I19" t="n">
-        <v>-0.05179</v>
+        <v>-0.04414</v>
       </c>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="n">
-        <v>1.01773</v>
+        <v>1.01207</v>
       </c>
       <c r="L19" t="n">
-        <v>-10.3108</v>
+        <v>-10.21487</v>
       </c>
     </row>
     <row r="20">
@@ -1151,13 +1151,13 @@
         <v>5</v>
       </c>
       <c r="C20" t="n">
-        <v>0.10664</v>
+        <v>0.26638</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.05175</v>
+        <v>-0.05246</v>
       </c>
       <c r="E20" t="n">
-        <v>0.07597</v>
+        <v>0.07678</v>
       </c>
       <c r="F20" t="n">
         <v>-0.076</v>
@@ -1166,17 +1166,17 @@
         <v>-0.016</v>
       </c>
       <c r="H20" t="n">
-        <v>-0.02425</v>
+        <v>-0.02354</v>
       </c>
       <c r="I20" t="n">
-        <v>-0.09197</v>
+        <v>-0.09278</v>
       </c>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="n">
-        <v>1.01957</v>
+        <v>1.01645</v>
       </c>
       <c r="L20" t="n">
-        <v>-8.771990000000001</v>
+        <v>-8.74832</v>
       </c>
     </row>
     <row r="21">
@@ -1187,32 +1187,32 @@
         <v>6</v>
       </c>
       <c r="C21" t="n">
-        <v>0.10664</v>
+        <v>0.26638</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.1135</v>
+        <v>-0.1129</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.0122</v>
+        <v>0.32132</v>
       </c>
       <c r="F21" t="n">
         <v>-0.112</v>
       </c>
       <c r="G21" t="n">
-        <v>0.08387</v>
+        <v>0.165</v>
       </c>
       <c r="H21" t="n">
-        <v>0.0015</v>
+        <v>0.0009</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>-0.15632</v>
       </c>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="n">
-        <v>1.07</v>
+        <v>1.0748</v>
       </c>
       <c r="L21" t="n">
-        <v>-14.21773</v>
+        <v>-14.39497</v>
       </c>
     </row>
     <row r="22">
@@ -1223,13 +1223,13 @@
         <v>7</v>
       </c>
       <c r="C22" t="n">
-        <v>0.10664</v>
+        <v>0.26638</v>
       </c>
       <c r="D22" t="n">
-        <v>0.00087</v>
+        <v>-0.00625</v>
       </c>
       <c r="E22" t="n">
-        <v>0.10664</v>
+        <v>0.009679999999999999</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -1238,17 +1238,17 @@
         <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>-0.00087</v>
+        <v>0.00625</v>
       </c>
       <c r="I22" t="n">
-        <v>-0.10664</v>
+        <v>-0.009679999999999999</v>
       </c>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="n">
-        <v>1.06162</v>
+        <v>1.03385</v>
       </c>
       <c r="L22" t="n">
-        <v>-13.35855</v>
+        <v>-13.23109</v>
       </c>
     </row>
     <row r="23">
@@ -1259,32 +1259,32 @@
         <v>8</v>
       </c>
       <c r="C23" t="n">
-        <v>0.10664</v>
+        <v>0.26638</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="E23" t="n">
-        <v>0.11103</v>
+        <v>-0.32638</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>0.55691</v>
+        <v>-0.06</v>
       </c>
       <c r="H23" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>0.26638</v>
       </c>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="n">
-        <v>1.09</v>
+        <v>1.02844</v>
       </c>
       <c r="L23" t="n">
-        <v>-13.35855</v>
+        <v>-13.23109</v>
       </c>
     </row>
     <row r="24">
@@ -1295,13 +1295,13 @@
         <v>9</v>
       </c>
       <c r="C24" t="n">
-        <v>0.10664</v>
+        <v>0.26638</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.31751</v>
+        <v>-0.28407</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.15917</v>
+        <v>-0.13485</v>
       </c>
       <c r="F24" t="n">
         <v>-0.295</v>
@@ -1310,17 +1310,17 @@
         <v>-0.166</v>
       </c>
       <c r="H24" t="n">
-        <v>0.02251</v>
+        <v>-0.01093</v>
       </c>
       <c r="I24" t="n">
-        <v>-0.00683</v>
+        <v>-0.03115</v>
       </c>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="n">
-        <v>1.05601</v>
+        <v>1.03789</v>
       </c>
       <c r="L24" t="n">
-        <v>-14.93808</v>
+        <v>-14.81493</v>
       </c>
     </row>
     <row r="25">
@@ -1331,13 +1331,13 @@
         <v>10</v>
       </c>
       <c r="C25" t="n">
-        <v>0.10664</v>
+        <v>0.26638</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.09062000000000001</v>
+        <v>-0.08676</v>
       </c>
       <c r="E25" t="n">
-        <v>-0.05758</v>
+        <v>-0.05909</v>
       </c>
       <c r="F25" t="n">
         <v>-0.09</v>
@@ -1346,17 +1346,17 @@
         <v>-0.058</v>
       </c>
       <c r="H25" t="n">
-        <v>0.00062</v>
+        <v>-0.00324</v>
       </c>
       <c r="I25" t="n">
-        <v>-0.00042</v>
+        <v>0.00109</v>
       </c>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="n">
-        <v>1.05105</v>
+        <v>1.03688</v>
       </c>
       <c r="L25" t="n">
-        <v>-15.09619</v>
+        <v>-15.0184</v>
       </c>
     </row>
     <row r="26">
@@ -1367,13 +1367,13 @@
         <v>11</v>
       </c>
       <c r="C26" t="n">
-        <v>0.10664</v>
+        <v>0.26638</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.03465</v>
+        <v>-0.03519</v>
       </c>
       <c r="E26" t="n">
-        <v>-0.01764</v>
+        <v>-0.01788</v>
       </c>
       <c r="F26" t="n">
         <v>-0.035</v>
@@ -1382,17 +1382,17 @@
         <v>-0.018</v>
       </c>
       <c r="H26" t="n">
-        <v>-0.00035</v>
+        <v>0.00019</v>
       </c>
       <c r="I26" t="n">
-        <v>-0.00036</v>
+        <v>-0.00012</v>
       </c>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="n">
-        <v>1.05694</v>
+        <v>1.05206</v>
       </c>
       <c r="L26" t="n">
-        <v>-14.78827</v>
+        <v>-14.82105</v>
       </c>
     </row>
     <row r="27">
@@ -1403,13 +1403,13 @@
         <v>12</v>
       </c>
       <c r="C27" t="n">
-        <v>0.10664</v>
+        <v>0.26638</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.05933</v>
+        <v>-0.06173</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.01479</v>
+        <v>-0.01517</v>
       </c>
       <c r="F27" t="n">
         <v>-0.061</v>
@@ -1418,17 +1418,17 @@
         <v>-0.016</v>
       </c>
       <c r="H27" t="n">
-        <v>-0.00167</v>
+        <v>0.00073</v>
       </c>
       <c r="I27" t="n">
-        <v>-0.00121</v>
+        <v>-0.00083</v>
       </c>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="n">
-        <v>1.0552</v>
+        <v>1.05833</v>
       </c>
       <c r="L27" t="n">
-        <v>-15.07238</v>
+        <v>-15.23851</v>
       </c>
     </row>
     <row r="28">
@@ -1439,13 +1439,13 @@
         <v>13</v>
       </c>
       <c r="C28" t="n">
-        <v>0.10664</v>
+        <v>0.26638</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.13411</v>
+        <v>-0.13697</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.05668</v>
+        <v>-0.05527</v>
       </c>
       <c r="F28" t="n">
         <v>-0.135</v>
@@ -1454,17 +1454,17 @@
         <v>-0.058</v>
       </c>
       <c r="H28" t="n">
-        <v>-0.0008899999999999999</v>
+        <v>0.00197</v>
       </c>
       <c r="I28" t="n">
-        <v>-0.00132</v>
+        <v>-0.00273</v>
       </c>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="n">
-        <v>1.05039</v>
+        <v>1.05191</v>
       </c>
       <c r="L28" t="n">
-        <v>-15.15328</v>
+        <v>-15.27675</v>
       </c>
     </row>
     <row r="29">
@@ -1475,13 +1475,13 @@
         <v>14</v>
       </c>
       <c r="C29" t="n">
-        <v>0.10664</v>
+        <v>0.26638</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.1496</v>
+        <v>-0.14461</v>
       </c>
       <c r="E29" t="n">
-        <v>-0.04862</v>
+        <v>-0.05079</v>
       </c>
       <c r="F29" t="n">
         <v>-0.149</v>
@@ -1490,17 +1490,17 @@
         <v>-0.05</v>
       </c>
       <c r="H29" t="n">
-        <v>0.0005999999999999999</v>
+        <v>-0.00439</v>
       </c>
       <c r="I29" t="n">
-        <v>-0.00138</v>
+        <v>0.00079</v>
       </c>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="n">
-        <v>1.03558</v>
+        <v>1.02585</v>
       </c>
       <c r="L29" t="n">
-        <v>-16.03177</v>
+        <v>-16.02996</v>
       </c>
     </row>
     <row r="30">
@@ -1511,19 +1511,19 @@
         <v>1</v>
       </c>
       <c r="C30" t="n">
-        <v>0.00105</v>
+        <v>0.03385</v>
       </c>
       <c r="D30" t="n">
-        <v>2.32327</v>
+        <v>2.32373</v>
       </c>
       <c r="E30" t="n">
-        <v>-0.16561</v>
+        <v>-0.15138</v>
       </c>
       <c r="F30" t="n">
         <v>2.324</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.17688</v>
+        <v>-0.14566</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
@@ -1547,22 +1547,22 @@
         <v>2</v>
       </c>
       <c r="C31" t="n">
-        <v>0.00105</v>
+        <v>0.03385</v>
       </c>
       <c r="D31" t="n">
-        <v>0.1831</v>
+        <v>0.18309</v>
       </c>
       <c r="E31" t="n">
-        <v>0.30782</v>
+        <v>0.35925</v>
       </c>
       <c r="F31" t="n">
         <v>0.183</v>
       </c>
       <c r="G31" t="n">
-        <v>0.20529</v>
+        <v>0.32852</v>
       </c>
       <c r="H31" t="n">
-        <v>-0.0001</v>
+        <v>-9.000000000000001e-05</v>
       </c>
       <c r="I31" t="n">
         <v>0</v>
@@ -1572,7 +1572,7 @@
         <v>1.045</v>
       </c>
       <c r="L31" t="n">
-        <v>-4.98259</v>
+        <v>-4.99269</v>
       </c>
     </row>
     <row r="32">
@@ -1583,22 +1583,22 @@
         <v>3</v>
       </c>
       <c r="C32" t="n">
-        <v>0.00105</v>
+        <v>0.03385</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.94189</v>
+        <v>-0.94199</v>
       </c>
       <c r="E32" t="n">
-        <v>0.06038</v>
+        <v>0.09429999999999999</v>
       </c>
       <c r="F32" t="n">
         <v>-0.9419999999999999</v>
       </c>
       <c r="G32" t="n">
-        <v>0.01604</v>
+        <v>0.09772</v>
       </c>
       <c r="H32" t="n">
-        <v>-0.00011</v>
+        <v>-1e-05</v>
       </c>
       <c r="I32" t="n">
         <v>0</v>
@@ -1608,7 +1608,7 @@
         <v>1.01</v>
       </c>
       <c r="L32" t="n">
-        <v>-12.7251</v>
+        <v>-12.76809</v>
       </c>
     </row>
     <row r="33">
@@ -1619,13 +1619,13 @@
         <v>4</v>
       </c>
       <c r="C33" t="n">
-        <v>0.00105</v>
+        <v>0.03385</v>
       </c>
       <c r="D33" t="n">
-        <v>-0.47761</v>
+        <v>-0.47746</v>
       </c>
       <c r="E33" t="n">
-        <v>0.03936</v>
+        <v>0.039</v>
       </c>
       <c r="F33" t="n">
         <v>-0.478</v>
@@ -1634,17 +1634,17 @@
         <v>0.039</v>
       </c>
       <c r="H33" t="n">
-        <v>-0.00039</v>
+        <v>-0.00054</v>
       </c>
       <c r="I33" t="n">
-        <v>-0.00036</v>
+        <v>-0</v>
       </c>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="n">
-        <v>1.01767</v>
+        <v>1.01038</v>
       </c>
       <c r="L33" t="n">
-        <v>-10.3129</v>
+        <v>-10.20464</v>
       </c>
     </row>
     <row r="34">
@@ -1655,13 +1655,13 @@
         <v>5</v>
       </c>
       <c r="C34" t="n">
-        <v>0.00105</v>
+        <v>0.03385</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.07587000000000001</v>
+        <v>-0.07562000000000001</v>
       </c>
       <c r="E34" t="n">
-        <v>-0.01536</v>
+        <v>-0.0156</v>
       </c>
       <c r="F34" t="n">
         <v>-0.076</v>
@@ -1670,17 +1670,17 @@
         <v>-0.016</v>
       </c>
       <c r="H34" t="n">
-        <v>-0.00013</v>
+        <v>-0.00038</v>
       </c>
       <c r="I34" t="n">
-        <v>-0.0006400000000000001</v>
+        <v>-0.0004</v>
       </c>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="n">
-        <v>1.01951</v>
+        <v>1.01501</v>
       </c>
       <c r="L34" t="n">
-        <v>-8.773849999999999</v>
+        <v>-8.741440000000001</v>
       </c>
     </row>
     <row r="35">
@@ -1691,32 +1691,32 @@
         <v>6</v>
       </c>
       <c r="C35" t="n">
-        <v>0.00105</v>
+        <v>0.03385</v>
       </c>
       <c r="D35" t="n">
-        <v>-0.11194</v>
+        <v>-0.11213</v>
       </c>
       <c r="E35" t="n">
-        <v>0.05175</v>
+        <v>0.16704</v>
       </c>
       <c r="F35" t="n">
         <v>-0.112</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.0122</v>
+        <v>0.165</v>
       </c>
       <c r="H35" t="n">
-        <v>-6e-05</v>
+        <v>0.00013</v>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>-0.00204</v>
       </c>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="n">
-        <v>1.07</v>
+        <v>1.07154</v>
       </c>
       <c r="L35" t="n">
-        <v>-14.22095</v>
+        <v>-14.43076</v>
       </c>
     </row>
     <row r="36">
@@ -1727,13 +1727,13 @@
         <v>7</v>
       </c>
       <c r="C36" t="n">
-        <v>0.00105</v>
+        <v>0.03385</v>
       </c>
       <c r="D36" t="n">
-        <v>2e-05</v>
+        <v>0.00039</v>
       </c>
       <c r="E36" t="n">
-        <v>0.00105</v>
+        <v>-0.00032</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
@@ -1742,17 +1742,17 @@
         <v>0</v>
       </c>
       <c r="H36" t="n">
-        <v>-2e-05</v>
+        <v>-0.00039</v>
       </c>
       <c r="I36" t="n">
-        <v>-0.00105</v>
+        <v>0.00032</v>
       </c>
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="n">
-        <v>1.06152</v>
+        <v>1.02811</v>
       </c>
       <c r="L36" t="n">
-        <v>-13.35963</v>
+        <v>-13.23752</v>
       </c>
     </row>
     <row r="37">
@@ -1763,32 +1763,32 @@
         <v>8</v>
       </c>
       <c r="C37" t="n">
-        <v>0.00105</v>
+        <v>0.03385</v>
       </c>
       <c r="D37" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>0.17562</v>
+        <v>-0.03157</v>
       </c>
       <c r="F37" t="n">
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>0.11103</v>
+        <v>-0.06</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>-0.02843</v>
       </c>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="n">
-        <v>1.09</v>
+        <v>1.01778</v>
       </c>
       <c r="L37" t="n">
-        <v>-13.35963</v>
+        <v>-13.23752</v>
       </c>
     </row>
     <row r="38">
@@ -1799,13 +1799,13 @@
         <v>9</v>
       </c>
       <c r="C38" t="n">
-        <v>0.00105</v>
+        <v>0.03385</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.29535</v>
+        <v>-0.29567</v>
       </c>
       <c r="E38" t="n">
-        <v>-0.16589</v>
+        <v>-0.16637</v>
       </c>
       <c r="F38" t="n">
         <v>-0.295</v>
@@ -1814,17 +1814,17 @@
         <v>-0.166</v>
       </c>
       <c r="H38" t="n">
-        <v>0.00035</v>
+        <v>0.00067</v>
       </c>
       <c r="I38" t="n">
-        <v>-0.00011</v>
+        <v>0.00037</v>
       </c>
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="n">
-        <v>1.05593</v>
+        <v>1.0331</v>
       </c>
       <c r="L38" t="n">
-        <v>-14.93852</v>
+        <v>-14.83244</v>
       </c>
     </row>
     <row r="39">
@@ -1835,13 +1835,13 @@
         <v>10</v>
       </c>
       <c r="C39" t="n">
-        <v>0.00105</v>
+        <v>0.03385</v>
       </c>
       <c r="D39" t="n">
-        <v>-0.08996999999999999</v>
+        <v>-0.08978999999999999</v>
       </c>
       <c r="E39" t="n">
-        <v>-0.058</v>
+        <v>-0.05803</v>
       </c>
       <c r="F39" t="n">
         <v>-0.09</v>
@@ -1850,17 +1850,17 @@
         <v>-0.058</v>
       </c>
       <c r="H39" t="n">
-        <v>-3e-05</v>
+        <v>-0.00021</v>
       </c>
       <c r="I39" t="n">
-        <v>-0</v>
+        <v>3e-05</v>
       </c>
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="n">
-        <v>1.05098</v>
+        <v>1.03232</v>
       </c>
       <c r="L39" t="n">
-        <v>-15.09729</v>
+        <v>-15.0425</v>
       </c>
     </row>
     <row r="40">
@@ -1871,13 +1871,13 @@
         <v>11</v>
       </c>
       <c r="C40" t="n">
-        <v>0.00105</v>
+        <v>0.03385</v>
       </c>
       <c r="D40" t="n">
-        <v>-0.03495</v>
+        <v>-0.03455</v>
       </c>
       <c r="E40" t="n">
-        <v>-0.01801</v>
+        <v>-0.01813</v>
       </c>
       <c r="F40" t="n">
         <v>-0.035</v>
@@ -1886,17 +1886,17 @@
         <v>-0.018</v>
       </c>
       <c r="H40" t="n">
-        <v>-5e-05</v>
+        <v>-0.00045</v>
       </c>
       <c r="I40" t="n">
-        <v>1e-05</v>
+        <v>0.00013</v>
       </c>
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="n">
-        <v>1.05691</v>
+        <v>1.04811</v>
       </c>
       <c r="L40" t="n">
-        <v>-14.79062</v>
+        <v>-14.85345</v>
       </c>
     </row>
     <row r="41">
@@ -1907,13 +1907,13 @@
         <v>12</v>
       </c>
       <c r="C41" t="n">
-        <v>0.00105</v>
+        <v>0.03385</v>
       </c>
       <c r="D41" t="n">
-        <v>-0.061</v>
+        <v>-0.06101</v>
       </c>
       <c r="E41" t="n">
-        <v>-0.016</v>
+        <v>-0.01597</v>
       </c>
       <c r="F41" t="n">
         <v>-0.061</v>
@@ -1922,17 +1922,17 @@
         <v>-0.016</v>
       </c>
       <c r="H41" t="n">
-        <v>-0</v>
+        <v>1e-05</v>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>-3e-05</v>
       </c>
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="n">
-        <v>1.05519</v>
+        <v>1.0549</v>
       </c>
       <c r="L41" t="n">
-        <v>-15.07558</v>
+        <v>-15.27984</v>
       </c>
     </row>
     <row r="42">
@@ -1943,13 +1943,13 @@
         <v>13</v>
       </c>
       <c r="C42" t="n">
-        <v>0.00105</v>
+        <v>0.03385</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.13497</v>
+        <v>-0.13478</v>
       </c>
       <c r="E42" t="n">
-        <v>-0.058</v>
+        <v>-0.05806</v>
       </c>
       <c r="F42" t="n">
         <v>-0.135</v>
@@ -1958,17 +1958,17 @@
         <v>-0.058</v>
       </c>
       <c r="H42" t="n">
-        <v>-3e-05</v>
+        <v>-0.00022</v>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>6e-05</v>
       </c>
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="n">
-        <v>1.05038</v>
+        <v>1.04835</v>
       </c>
       <c r="L42" t="n">
-        <v>-15.15628</v>
+        <v>-15.31667</v>
       </c>
     </row>
     <row r="43">
@@ -1979,13 +1979,13 @@
         <v>14</v>
       </c>
       <c r="C43" t="n">
-        <v>0.00105</v>
+        <v>0.03385</v>
       </c>
       <c r="D43" t="n">
-        <v>-0.14897</v>
+        <v>-0.14876</v>
       </c>
       <c r="E43" t="n">
-        <v>-0.05</v>
+        <v>-0.05008</v>
       </c>
       <c r="F43" t="n">
         <v>-0.149</v>
@@ -1994,17 +1994,1025 @@
         <v>-0.05</v>
       </c>
       <c r="H43" t="n">
-        <v>-3e-05</v>
+        <v>-0.00024</v>
       </c>
       <c r="I43" t="n">
-        <v>-0</v>
+        <v>8.000000000000001e-05</v>
       </c>
       <c r="J43" t="inlineStr"/>
       <c r="K43" t="n">
-        <v>1.03553</v>
+        <v>1.02151</v>
       </c>
       <c r="L43" t="n">
-        <v>-16.03364</v>
+        <v>-16.06782</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>4</v>
+      </c>
+      <c r="B44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.02811</v>
+      </c>
+      <c r="D44" t="n">
+        <v>2.3261</v>
+      </c>
+      <c r="E44" t="n">
+        <v>-0.14526</v>
+      </c>
+      <c r="F44" t="n">
+        <v>2.324</v>
+      </c>
+      <c r="G44" t="n">
+        <v>-0.15138</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" t="inlineStr"/>
+      <c r="K44" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="L44" t="n">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>4</v>
+      </c>
+      <c r="B45" t="n">
+        <v>2</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.02811</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.18301</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.37815</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.183</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.35925</v>
+      </c>
+      <c r="H45" t="n">
+        <v>-1e-05</v>
+      </c>
+      <c r="I45" t="n">
+        <v>-0.0189</v>
+      </c>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="n">
+        <v>1.04432</v>
+      </c>
+      <c r="L45" t="n">
+        <v>-4.98379</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>4</v>
+      </c>
+      <c r="B46" t="n">
+        <v>3</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.02811</v>
+      </c>
+      <c r="D46" t="n">
+        <v>-0.9419999999999999</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.10446</v>
+      </c>
+      <c r="F46" t="n">
+        <v>-0.9419999999999999</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.09429999999999999</v>
+      </c>
+      <c r="H46" t="n">
+        <v>-0</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" t="inlineStr"/>
+      <c r="K46" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="L46" t="n">
+        <v>-12.77617</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>4</v>
+      </c>
+      <c r="B47" t="n">
+        <v>4</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.02811</v>
+      </c>
+      <c r="D47" t="n">
+        <v>-0.47801</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.039</v>
+      </c>
+      <c r="F47" t="n">
+        <v>-0.478</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.039</v>
+      </c>
+      <c r="H47" t="n">
+        <v>1e-05</v>
+      </c>
+      <c r="I47" t="n">
+        <v>-0</v>
+      </c>
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="n">
+        <v>1.00997</v>
+      </c>
+      <c r="L47" t="n">
+        <v>-10.20503</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>4</v>
+      </c>
+      <c r="B48" t="n">
+        <v>5</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.02811</v>
+      </c>
+      <c r="D48" t="n">
+        <v>-0.07600999999999999</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-0.016</v>
+      </c>
+      <c r="F48" t="n">
+        <v>-0.076</v>
+      </c>
+      <c r="G48" t="n">
+        <v>-0.016</v>
+      </c>
+      <c r="H48" t="n">
+        <v>1e-05</v>
+      </c>
+      <c r="I48" t="n">
+        <v>-0</v>
+      </c>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="n">
+        <v>1.01461</v>
+      </c>
+      <c r="L48" t="n">
+        <v>-8.740729999999999</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>4</v>
+      </c>
+      <c r="B49" t="n">
+        <v>6</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.02811</v>
+      </c>
+      <c r="D49" t="n">
+        <v>-0.112</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.16501</v>
+      </c>
+      <c r="F49" t="n">
+        <v>-0.112</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0.165</v>
+      </c>
+      <c r="H49" t="n">
+        <v>-0</v>
+      </c>
+      <c r="I49" t="n">
+        <v>-1e-05</v>
+      </c>
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="n">
+        <v>1.07108</v>
+      </c>
+      <c r="L49" t="n">
+        <v>-14.43515</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>4</v>
+      </c>
+      <c r="B50" t="n">
+        <v>7</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.02811</v>
+      </c>
+      <c r="D50" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E50" t="n">
+        <v>-0</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="n">
+        <v>1.02763</v>
+      </c>
+      <c r="L50" t="n">
+        <v>-13.24057</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>4</v>
+      </c>
+      <c r="B51" t="n">
+        <v>8</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.02811</v>
+      </c>
+      <c r="D51" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E51" t="n">
+        <v>-0.0597</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" t="n">
+        <v>-0.0003</v>
+      </c>
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="n">
+        <v>1.01724</v>
+      </c>
+      <c r="L51" t="n">
+        <v>-13.24057</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>4</v>
+      </c>
+      <c r="B52" t="n">
+        <v>9</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.02811</v>
+      </c>
+      <c r="D52" t="n">
+        <v>-0.295</v>
+      </c>
+      <c r="E52" t="n">
+        <v>-0.16599</v>
+      </c>
+      <c r="F52" t="n">
+        <v>-0.295</v>
+      </c>
+      <c r="G52" t="n">
+        <v>-0.166</v>
+      </c>
+      <c r="H52" t="n">
+        <v>-0</v>
+      </c>
+      <c r="I52" t="n">
+        <v>-1e-05</v>
+      </c>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="n">
+        <v>1.03261</v>
+      </c>
+      <c r="L52" t="n">
+        <v>-14.83703</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>4</v>
+      </c>
+      <c r="B53" t="n">
+        <v>10</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.02811</v>
+      </c>
+      <c r="D53" t="n">
+        <v>-0.08999</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-0.058</v>
+      </c>
+      <c r="F53" t="n">
+        <v>-0.09</v>
+      </c>
+      <c r="G53" t="n">
+        <v>-0.058</v>
+      </c>
+      <c r="H53" t="n">
+        <v>-1e-05</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" t="inlineStr"/>
+      <c r="K53" t="n">
+        <v>1.03184</v>
+      </c>
+      <c r="L53" t="n">
+        <v>-15.04734</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>4</v>
+      </c>
+      <c r="B54" t="n">
+        <v>11</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.02811</v>
+      </c>
+      <c r="D54" t="n">
+        <v>-0.035</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-0.018</v>
+      </c>
+      <c r="F54" t="n">
+        <v>-0.035</v>
+      </c>
+      <c r="G54" t="n">
+        <v>-0.018</v>
+      </c>
+      <c r="H54" t="n">
+        <v>-0</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0</v>
+      </c>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="n">
+        <v>1.04764</v>
+      </c>
+      <c r="L54" t="n">
+        <v>-14.85818</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>4</v>
+      </c>
+      <c r="B55" t="n">
+        <v>12</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.02811</v>
+      </c>
+      <c r="D55" t="n">
+        <v>-0.061</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-0.016</v>
+      </c>
+      <c r="F55" t="n">
+        <v>-0.061</v>
+      </c>
+      <c r="G55" t="n">
+        <v>-0.016</v>
+      </c>
+      <c r="H55" t="n">
+        <v>-0</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" t="inlineStr"/>
+      <c r="K55" t="n">
+        <v>1.05443</v>
+      </c>
+      <c r="L55" t="n">
+        <v>-15.28501</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>4</v>
+      </c>
+      <c r="B56" t="n">
+        <v>13</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.02811</v>
+      </c>
+      <c r="D56" t="n">
+        <v>-0.135</v>
+      </c>
+      <c r="E56" t="n">
+        <v>-0.058</v>
+      </c>
+      <c r="F56" t="n">
+        <v>-0.135</v>
+      </c>
+      <c r="G56" t="n">
+        <v>-0.058</v>
+      </c>
+      <c r="H56" t="n">
+        <v>-0</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" t="inlineStr"/>
+      <c r="K56" t="n">
+        <v>1.04788</v>
+      </c>
+      <c r="L56" t="n">
+        <v>-15.32186</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>4</v>
+      </c>
+      <c r="B57" t="n">
+        <v>14</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.02811</v>
+      </c>
+      <c r="D57" t="n">
+        <v>-0.14899</v>
+      </c>
+      <c r="E57" t="n">
+        <v>-0.05</v>
+      </c>
+      <c r="F57" t="n">
+        <v>-0.149</v>
+      </c>
+      <c r="G57" t="n">
+        <v>-0.05</v>
+      </c>
+      <c r="H57" t="n">
+        <v>-1e-05</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="n">
+        <v>1.02102</v>
+      </c>
+      <c r="L57" t="n">
+        <v>-16.07371</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>5</v>
+      </c>
+      <c r="B58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.02763</v>
+      </c>
+      <c r="D58" t="n">
+        <v>2.32613</v>
+      </c>
+      <c r="E58" t="n">
+        <v>-0.13154</v>
+      </c>
+      <c r="F58" t="n">
+        <v>2.324</v>
+      </c>
+      <c r="G58" t="n">
+        <v>-0.14526</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" t="inlineStr"/>
+      <c r="K58" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="L58" t="n">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>5</v>
+      </c>
+      <c r="B59" t="n">
+        <v>2</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.02763</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.183</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.35927</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.183</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0.373</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0.01373</v>
+      </c>
+      <c r="J59" t="inlineStr"/>
+      <c r="K59" t="n">
+        <v>1.04481</v>
+      </c>
+      <c r="L59" t="n">
+        <v>-4.99027</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>5</v>
+      </c>
+      <c r="B60" t="n">
+        <v>3</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.02763</v>
+      </c>
+      <c r="D60" t="n">
+        <v>-0.9419999999999999</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.11048</v>
+      </c>
+      <c r="F60" t="n">
+        <v>-0.9419999999999999</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0.10446</v>
+      </c>
+      <c r="H60" t="n">
+        <v>-0</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" t="inlineStr"/>
+      <c r="K60" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="L60" t="n">
+        <v>-12.77052</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>5</v>
+      </c>
+      <c r="B61" t="n">
+        <v>4</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.02763</v>
+      </c>
+      <c r="D61" t="n">
+        <v>-0.478</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.039</v>
+      </c>
+      <c r="F61" t="n">
+        <v>-0.478</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0.039</v>
+      </c>
+      <c r="H61" t="n">
+        <v>-0</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" t="inlineStr"/>
+      <c r="K61" t="n">
+        <v>1.01025</v>
+      </c>
+      <c r="L61" t="n">
+        <v>-10.20466</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>5</v>
+      </c>
+      <c r="B62" t="n">
+        <v>5</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0.02763</v>
+      </c>
+      <c r="D62" t="n">
+        <v>-0.076</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-0.016</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-0.076</v>
+      </c>
+      <c r="G62" t="n">
+        <v>-0.016</v>
+      </c>
+      <c r="H62" t="n">
+        <v>-0</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0</v>
+      </c>
+      <c r="J62" t="inlineStr"/>
+      <c r="K62" t="n">
+        <v>1.01489</v>
+      </c>
+      <c r="L62" t="n">
+        <v>-8.74119</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>5</v>
+      </c>
+      <c r="B63" t="n">
+        <v>6</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0.02763</v>
+      </c>
+      <c r="D63" t="n">
+        <v>-0.112</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.165</v>
+      </c>
+      <c r="F63" t="n">
+        <v>-0.112</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0.165</v>
+      </c>
+      <c r="H63" t="n">
+        <v>-0</v>
+      </c>
+      <c r="I63" t="n">
+        <v>-0</v>
+      </c>
+      <c r="J63" t="inlineStr"/>
+      <c r="K63" t="n">
+        <v>1.07138</v>
+      </c>
+      <c r="L63" t="n">
+        <v>-14.43237</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>5</v>
+      </c>
+      <c r="B64" t="n">
+        <v>7</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0.02763</v>
+      </c>
+      <c r="D64" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-0</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0</v>
+      </c>
+      <c r="J64" t="inlineStr"/>
+      <c r="K64" t="n">
+        <v>1.02793</v>
+      </c>
+      <c r="L64" t="n">
+        <v>-13.23845</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>5</v>
+      </c>
+      <c r="B65" t="n">
+        <v>8</v>
+      </c>
+      <c r="C65" t="n">
+        <v>0.02763</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0</v>
+      </c>
+      <c r="G65" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="H65" t="n">
+        <v>-0</v>
+      </c>
+      <c r="I65" t="n">
+        <v>-0</v>
+      </c>
+      <c r="J65" t="inlineStr"/>
+      <c r="K65" t="n">
+        <v>1.01754</v>
+      </c>
+      <c r="L65" t="n">
+        <v>-13.23845</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>5</v>
+      </c>
+      <c r="B66" t="n">
+        <v>9</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0.02763</v>
+      </c>
+      <c r="D66" t="n">
+        <v>-0.295</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-0.166</v>
+      </c>
+      <c r="F66" t="n">
+        <v>-0.295</v>
+      </c>
+      <c r="G66" t="n">
+        <v>-0.166</v>
+      </c>
+      <c r="H66" t="n">
+        <v>-0</v>
+      </c>
+      <c r="I66" t="n">
+        <v>-0</v>
+      </c>
+      <c r="J66" t="inlineStr"/>
+      <c r="K66" t="n">
+        <v>1.03292</v>
+      </c>
+      <c r="L66" t="n">
+        <v>-14.83395</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>5</v>
+      </c>
+      <c r="B67" t="n">
+        <v>10</v>
+      </c>
+      <c r="C67" t="n">
+        <v>0.02763</v>
+      </c>
+      <c r="D67" t="n">
+        <v>-0.09</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-0.058</v>
+      </c>
+      <c r="F67" t="n">
+        <v>-0.09</v>
+      </c>
+      <c r="G67" t="n">
+        <v>-0.058</v>
+      </c>
+      <c r="H67" t="n">
+        <v>-0</v>
+      </c>
+      <c r="I67" t="n">
+        <v>-0</v>
+      </c>
+      <c r="J67" t="inlineStr"/>
+      <c r="K67" t="n">
+        <v>1.03215</v>
+      </c>
+      <c r="L67" t="n">
+        <v>-15.04415</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>5</v>
+      </c>
+      <c r="B68" t="n">
+        <v>11</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0.02763</v>
+      </c>
+      <c r="D68" t="n">
+        <v>-0.035</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-0.018</v>
+      </c>
+      <c r="F68" t="n">
+        <v>-0.035</v>
+      </c>
+      <c r="G68" t="n">
+        <v>-0.018</v>
+      </c>
+      <c r="H68" t="n">
+        <v>-0</v>
+      </c>
+      <c r="I68" t="n">
+        <v>0</v>
+      </c>
+      <c r="J68" t="inlineStr"/>
+      <c r="K68" t="n">
+        <v>1.04795</v>
+      </c>
+      <c r="L68" t="n">
+        <v>-14.85513</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>5</v>
+      </c>
+      <c r="B69" t="n">
+        <v>12</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0.02763</v>
+      </c>
+      <c r="D69" t="n">
+        <v>-0.061</v>
+      </c>
+      <c r="E69" t="n">
+        <v>-0.016</v>
+      </c>
+      <c r="F69" t="n">
+        <v>-0.061</v>
+      </c>
+      <c r="G69" t="n">
+        <v>-0.016</v>
+      </c>
+      <c r="H69" t="n">
+        <v>-0</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J69" t="inlineStr"/>
+      <c r="K69" t="n">
+        <v>1.05474</v>
+      </c>
+      <c r="L69" t="n">
+        <v>-15.28174</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>5</v>
+      </c>
+      <c r="B70" t="n">
+        <v>13</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0.02763</v>
+      </c>
+      <c r="D70" t="n">
+        <v>-0.135</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-0.058</v>
+      </c>
+      <c r="F70" t="n">
+        <v>-0.135</v>
+      </c>
+      <c r="G70" t="n">
+        <v>-0.058</v>
+      </c>
+      <c r="H70" t="n">
+        <v>-0</v>
+      </c>
+      <c r="I70" t="n">
+        <v>0</v>
+      </c>
+      <c r="J70" t="inlineStr"/>
+      <c r="K70" t="n">
+        <v>1.04819</v>
+      </c>
+      <c r="L70" t="n">
+        <v>-15.31855</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>5</v>
+      </c>
+      <c r="B71" t="n">
+        <v>14</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0.02763</v>
+      </c>
+      <c r="D71" t="n">
+        <v>-0.149</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-0.05</v>
+      </c>
+      <c r="F71" t="n">
+        <v>-0.149</v>
+      </c>
+      <c r="G71" t="n">
+        <v>-0.05</v>
+      </c>
+      <c r="H71" t="n">
+        <v>-0</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0</v>
+      </c>
+      <c r="J71" t="inlineStr"/>
+      <c r="K71" t="n">
+        <v>1.02134</v>
+      </c>
+      <c r="L71" t="n">
+        <v>-16.06991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualizadas algumas informações do controle
</commit_message>
<xml_diff>
--- a/relatorio_iteracoes_NR.xlsx
+++ b/relatorio_iteracoes_NR.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L71"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,13 +503,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>1.22044</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="D2" t="n">
-        <v>0.12298</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.36494</v>
+        <v>-0.051</v>
       </c>
       <c r="F2" t="n">
         <v>2.324</v>
@@ -525,7 +525,7 @@
       </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="n">
-        <v>1.06</v>
+        <v>1</v>
       </c>
       <c r="L2" t="n">
         <v>-0</v>
@@ -539,13 +539,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>1.22044</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0534</v>
+        <v>-0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.12014</v>
+        <v>-0.08260000000000001</v>
       </c>
       <c r="F3" t="n">
         <v>0.183</v>
@@ -554,17 +554,17 @@
         <v>0.297</v>
       </c>
       <c r="H3" t="n">
-        <v>0.1296</v>
+        <v>0.183</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
       </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="n">
-        <v>1.045</v>
+        <v>1</v>
       </c>
       <c r="L3" t="n">
-        <v>-4.74283</v>
+        <v>-5.44124</v>
       </c>
     </row>
     <row r="4">
@@ -575,13 +575,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>1.22044</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.05818</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.24398</v>
+        <v>-0.0283</v>
       </c>
       <c r="F4" t="n">
         <v>-0.9419999999999999</v>
@@ -590,17 +590,17 @@
         <v>0.044</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.8838200000000001</v>
+        <v>-0.9419999999999999</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
       </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="n">
-        <v>1.01</v>
+        <v>1</v>
       </c>
       <c r="L4" t="n">
-        <v>-12.34593</v>
+        <v>-13.97862</v>
       </c>
     </row>
     <row r="5">
@@ -611,13 +611,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>1.22044</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.03343</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.06521</v>
+        <v>0.14595</v>
       </c>
       <c r="F5" t="n">
         <v>-0.478</v>
@@ -626,17 +626,17 @@
         <v>0.039</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.44457</v>
+        <v>-0.478</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.02621</v>
+        <v>-0.10695</v>
       </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="n">
-        <v>1.01042</v>
+        <v>0.98697</v>
       </c>
       <c r="L5" t="n">
-        <v>-9.80561</v>
+        <v>-11.09221</v>
       </c>
     </row>
     <row r="6">
@@ -647,13 +647,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>1.22044</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.07826</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.22077</v>
+        <v>0.26873</v>
       </c>
       <c r="F6" t="n">
         <v>-0.076</v>
@@ -662,17 +662,17 @@
         <v>-0.016</v>
       </c>
       <c r="H6" t="n">
-        <v>0.00226</v>
+        <v>-0.076</v>
       </c>
       <c r="I6" t="n">
-        <v>0.20477</v>
+        <v>-0.28473</v>
       </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="n">
-        <v>1.01936</v>
+        <v>0.99136</v>
       </c>
       <c r="L6" t="n">
-        <v>-8.48696</v>
+        <v>-9.61924</v>
       </c>
     </row>
     <row r="7">
@@ -683,32 +683,32 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>1.22044</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="D7" t="n">
-        <v>0.09351</v>
+        <v>-0.10682</v>
       </c>
       <c r="E7" t="n">
-        <v>0.08387</v>
+        <v>-0.5118200000000001</v>
       </c>
       <c r="F7" t="n">
         <v>-0.112</v>
       </c>
       <c r="G7" t="n">
-        <v>0.165</v>
+        <v>0.047</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.20551</v>
+        <v>-0.00518</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.03687</v>
+        <v>0.55882</v>
       </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="n">
-        <v>1.08848</v>
+        <v>1.08854</v>
       </c>
       <c r="L7" t="n">
-        <v>-14.31205</v>
+        <v>-15.70933</v>
       </c>
     </row>
     <row r="8">
@@ -719,13 +719,13 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>1.22044</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>-1.22044</v>
+        <v>-0.10757</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -737,14 +737,14 @@
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>1.22044</v>
+        <v>0.10757</v>
       </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="n">
         <v>1</v>
       </c>
       <c r="L8" t="n">
-        <v>-12.72817</v>
+        <v>-14.0804</v>
       </c>
     </row>
     <row r="9">
@@ -755,32 +755,32 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>1.22044</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.55691</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.06</v>
+        <v>0.174</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.38291</v>
+        <v>0.174</v>
       </c>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="n">
-        <v>0.93876</v>
+        <v>0.9664199999999999</v>
       </c>
       <c r="L9" t="n">
-        <v>-12.72817</v>
+        <v>-14.0804</v>
       </c>
     </row>
     <row r="10">
@@ -791,13 +791,13 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>1.22044</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="D10" t="n">
-        <v>0.05068</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0.45273</v>
+        <v>-0.24752</v>
       </c>
       <c r="F10" t="n">
         <v>-0.295</v>
@@ -806,17 +806,17 @@
         <v>-0.166</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.34568</v>
+        <v>-0.295</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.61873</v>
+        <v>0.08152</v>
       </c>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="n">
-        <v>1.02081</v>
+        <v>1.01615</v>
       </c>
       <c r="L10" t="n">
-        <v>-14.24512</v>
+        <v>-15.68773</v>
       </c>
     </row>
     <row r="11">
@@ -827,13 +827,13 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>1.22044</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.03237</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.08223999999999999</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
         <v>-0.09</v>
@@ -842,17 +842,17 @@
         <v>-0.058</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.05763</v>
+        <v>-0.09</v>
       </c>
       <c r="I11" t="n">
-        <v>0.02424</v>
+        <v>-0.058</v>
       </c>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="n">
-        <v>1.02516</v>
+        <v>1.0211</v>
       </c>
       <c r="L11" t="n">
-        <v>-14.51409</v>
+        <v>-15.9772</v>
       </c>
     </row>
     <row r="12">
@@ -863,13 +863,13 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>1.22044</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.01494</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.02833</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
         <v>-0.035</v>
@@ -878,17 +878,17 @@
         <v>-0.018</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.02006</v>
+        <v>-0.035</v>
       </c>
       <c r="I12" t="n">
-        <v>0.01033</v>
+        <v>-0.018</v>
       </c>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="n">
-        <v>1.05279</v>
+        <v>1.05056</v>
       </c>
       <c r="L12" t="n">
-        <v>-14.51353</v>
+        <v>-15.95706</v>
       </c>
     </row>
     <row r="13">
@@ -899,13 +899,13 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>1.22044</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="D13" t="n">
-        <v>0.05327</v>
+        <v>0.30072</v>
       </c>
       <c r="E13" t="n">
-        <v>0.04819</v>
+        <v>0.40655</v>
       </c>
       <c r="F13" t="n">
         <v>-0.061</v>
@@ -914,17 +914,17 @@
         <v>-0.016</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.11427</v>
+        <v>-0.36172</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.06419</v>
+        <v>-0.42255</v>
       </c>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="n">
         <v>1.07</v>
       </c>
       <c r="L13" t="n">
-        <v>-15.13733</v>
+        <v>-16.60005</v>
       </c>
     </row>
     <row r="14">
@@ -935,13 +935,13 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>1.22044</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.10063</v>
+        <v>-0.17423</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.14142</v>
+        <v>-0.15764</v>
       </c>
       <c r="F14" t="n">
         <v>-0.135</v>
@@ -950,17 +950,17 @@
         <v>-0.058</v>
       </c>
       <c r="H14" t="n">
-        <v>-0.03437</v>
+        <v>0.03923</v>
       </c>
       <c r="I14" t="n">
-        <v>0.08341999999999999</v>
+        <v>0.09964000000000001</v>
       </c>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="n">
-        <v>1.06151</v>
+        <v>1.0614</v>
       </c>
       <c r="L14" t="n">
-        <v>-15.11322</v>
+        <v>-16.58094</v>
       </c>
     </row>
     <row r="15">
@@ -971,13 +971,13 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>1.22044</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.046</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.09634</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
         <v>-0.149</v>
@@ -986,17 +986,17 @@
         <v>-0.05</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.103</v>
+        <v>-0.149</v>
       </c>
       <c r="I15" t="n">
-        <v>0.04634</v>
+        <v>-0.05</v>
       </c>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="n">
-        <v>1.0205</v>
+        <v>1.01743</v>
       </c>
       <c r="L15" t="n">
-        <v>-15.61139</v>
+        <v>-17.15578</v>
       </c>
     </row>
     <row r="16">
@@ -1007,19 +1007,19 @@
         <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>0.26638</v>
+        <v>0.10944</v>
       </c>
       <c r="D16" t="n">
-        <v>2.22805</v>
+        <v>2.19456</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.14566</v>
+        <v>-0.53059</v>
       </c>
       <c r="F16" t="n">
         <v>2.324</v>
       </c>
       <c r="G16" t="n">
-        <v>0.36494</v>
+        <v>-0.051</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="n">
-        <v>1.06</v>
+        <v>1</v>
       </c>
       <c r="L16" t="n">
         <v>-0</v>
@@ -1043,32 +1043,32 @@
         <v>2</v>
       </c>
       <c r="C17" t="n">
-        <v>0.26638</v>
+        <v>0.10944</v>
       </c>
       <c r="D17" t="n">
-        <v>0.21778</v>
+        <v>0.21923</v>
       </c>
       <c r="E17" t="n">
-        <v>0.32852</v>
+        <v>0.20774</v>
       </c>
       <c r="F17" t="n">
         <v>0.183</v>
       </c>
       <c r="G17" t="n">
-        <v>0.12014</v>
+        <v>-0.08260000000000001</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.03478</v>
+        <v>-0.03623</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
       </c>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="n">
-        <v>1.045</v>
+        <v>1</v>
       </c>
       <c r="L17" t="n">
-        <v>-4.98487</v>
+        <v>-5.85515</v>
       </c>
     </row>
     <row r="18">
@@ -1079,32 +1079,32 @@
         <v>3</v>
       </c>
       <c r="C18" t="n">
-        <v>0.26638</v>
+        <v>0.10944</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.92549</v>
+        <v>-0.92087</v>
       </c>
       <c r="E18" t="n">
-        <v>0.09772</v>
+        <v>0.36428</v>
       </c>
       <c r="F18" t="n">
         <v>-0.9419999999999999</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.24398</v>
+        <v>-0.0283</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.01651</v>
+        <v>-0.02113</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
       </c>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="n">
-        <v>1.01</v>
+        <v>1</v>
       </c>
       <c r="L18" t="n">
-        <v>-12.74759</v>
+        <v>-14.69008</v>
       </c>
     </row>
     <row r="19">
@@ -1115,13 +1115,13 @@
         <v>4</v>
       </c>
       <c r="C19" t="n">
-        <v>0.26638</v>
+        <v>0.10944</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.46791</v>
+        <v>-0.4514</v>
       </c>
       <c r="E19" t="n">
-        <v>0.08314000000000001</v>
+        <v>0.08903</v>
       </c>
       <c r="F19" t="n">
         <v>-0.478</v>
@@ -1130,17 +1130,17 @@
         <v>0.039</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.01009</v>
+        <v>-0.0266</v>
       </c>
       <c r="I19" t="n">
-        <v>-0.04414</v>
+        <v>-0.05003</v>
       </c>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="n">
-        <v>1.01207</v>
+        <v>0.98158</v>
       </c>
       <c r="L19" t="n">
-        <v>-10.21487</v>
+        <v>-11.6924</v>
       </c>
     </row>
     <row r="20">
@@ -1151,13 +1151,13 @@
         <v>5</v>
       </c>
       <c r="C20" t="n">
-        <v>0.26638</v>
+        <v>0.10944</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.05246</v>
+        <v>-0.01914</v>
       </c>
       <c r="E20" t="n">
-        <v>0.07678</v>
+        <v>0.09344</v>
       </c>
       <c r="F20" t="n">
         <v>-0.076</v>
@@ -1166,17 +1166,17 @@
         <v>-0.016</v>
       </c>
       <c r="H20" t="n">
-        <v>-0.02354</v>
+        <v>-0.05686</v>
       </c>
       <c r="I20" t="n">
-        <v>-0.09278</v>
+        <v>-0.10944</v>
       </c>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="n">
-        <v>1.01645</v>
+        <v>0.9845699999999999</v>
       </c>
       <c r="L20" t="n">
-        <v>-8.74832</v>
+        <v>-10.16982</v>
       </c>
     </row>
     <row r="21">
@@ -1187,32 +1187,32 @@
         <v>6</v>
       </c>
       <c r="C21" t="n">
-        <v>0.26638</v>
+        <v>0.10944</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.1129</v>
+        <v>-0.09862</v>
       </c>
       <c r="E21" t="n">
-        <v>0.32132</v>
+        <v>0.45638</v>
       </c>
       <c r="F21" t="n">
         <v>-0.112</v>
       </c>
       <c r="G21" t="n">
-        <v>0.165</v>
+        <v>0.35224</v>
       </c>
       <c r="H21" t="n">
-        <v>0.0009</v>
+        <v>-0.01338</v>
       </c>
       <c r="I21" t="n">
-        <v>-0.15632</v>
+        <v>-0.10414</v>
       </c>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="n">
-        <v>1.0748</v>
+        <v>1.08913</v>
       </c>
       <c r="L21" t="n">
-        <v>-14.39497</v>
+        <v>-16.3252</v>
       </c>
     </row>
     <row r="22">
@@ -1223,13 +1223,13 @@
         <v>7</v>
       </c>
       <c r="C22" t="n">
-        <v>0.26638</v>
+        <v>0.10944</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.00625</v>
+        <v>0.00752</v>
       </c>
       <c r="E22" t="n">
-        <v>0.009679999999999999</v>
+        <v>0.0102</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -1238,17 +1238,17 @@
         <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>0.00625</v>
+        <v>-0.00752</v>
       </c>
       <c r="I22" t="n">
-        <v>-0.009679999999999999</v>
+        <v>-0.0102</v>
       </c>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="n">
-        <v>1.03385</v>
+        <v>1</v>
       </c>
       <c r="L22" t="n">
-        <v>-13.23109</v>
+        <v>-14.70529</v>
       </c>
     </row>
     <row r="23">
@@ -1259,32 +1259,32 @@
         <v>8</v>
       </c>
       <c r="C23" t="n">
-        <v>0.26638</v>
+        <v>0.10944</v>
       </c>
       <c r="D23" t="n">
         <v>-0</v>
       </c>
       <c r="E23" t="n">
-        <v>-0.32638</v>
+        <v>-0.18425</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.06</v>
+        <v>-0.19065</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>0.26638</v>
+        <v>-0.0064</v>
       </c>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="n">
-        <v>1.02844</v>
+        <v>0.97523</v>
       </c>
       <c r="L23" t="n">
-        <v>-13.23109</v>
+        <v>-14.70529</v>
       </c>
     </row>
     <row r="24">
@@ -1295,13 +1295,13 @@
         <v>9</v>
       </c>
       <c r="C24" t="n">
-        <v>0.26638</v>
+        <v>0.10944</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.28407</v>
+        <v>-0.29458</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.13485</v>
+        <v>-0.1549</v>
       </c>
       <c r="F24" t="n">
         <v>-0.295</v>
@@ -1310,17 +1310,17 @@
         <v>-0.166</v>
       </c>
       <c r="H24" t="n">
-        <v>-0.01093</v>
+        <v>-0.00042</v>
       </c>
       <c r="I24" t="n">
-        <v>-0.03115</v>
+        <v>-0.0111</v>
       </c>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="n">
-        <v>1.03789</v>
+        <v>1.01465</v>
       </c>
       <c r="L24" t="n">
-        <v>-14.81493</v>
+        <v>-16.27269</v>
       </c>
     </row>
     <row r="25">
@@ -1331,13 +1331,13 @@
         <v>10</v>
       </c>
       <c r="C25" t="n">
-        <v>0.26638</v>
+        <v>0.10944</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.08676</v>
+        <v>-0.09279</v>
       </c>
       <c r="E25" t="n">
-        <v>-0.05909</v>
+        <v>-0.05873</v>
       </c>
       <c r="F25" t="n">
         <v>-0.09</v>
@@ -1346,17 +1346,17 @@
         <v>-0.058</v>
       </c>
       <c r="H25" t="n">
-        <v>-0.00324</v>
+        <v>0.00279</v>
       </c>
       <c r="I25" t="n">
-        <v>0.00109</v>
+        <v>0.00073</v>
       </c>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="n">
-        <v>1.03688</v>
+        <v>1.02014</v>
       </c>
       <c r="L25" t="n">
-        <v>-15.0184</v>
+        <v>-16.55157</v>
       </c>
     </row>
     <row r="26">
@@ -1367,13 +1367,13 @@
         <v>11</v>
       </c>
       <c r="C26" t="n">
-        <v>0.26638</v>
+        <v>0.10944</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.03519</v>
+        <v>-0.03836</v>
       </c>
       <c r="E26" t="n">
-        <v>-0.01788</v>
+        <v>-0.01809</v>
       </c>
       <c r="F26" t="n">
         <v>-0.035</v>
@@ -1382,17 +1382,17 @@
         <v>-0.018</v>
       </c>
       <c r="H26" t="n">
-        <v>0.00019</v>
+        <v>0.00336</v>
       </c>
       <c r="I26" t="n">
-        <v>-0.00012</v>
+        <v>9.000000000000001e-05</v>
       </c>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="n">
-        <v>1.05206</v>
+        <v>1.05051</v>
       </c>
       <c r="L26" t="n">
-        <v>-14.82105</v>
+        <v>-16.53455</v>
       </c>
     </row>
     <row r="27">
@@ -1403,13 +1403,13 @@
         <v>12</v>
       </c>
       <c r="C27" t="n">
-        <v>0.26638</v>
+        <v>0.10944</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.06173</v>
+        <v>-0.06551</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.01517</v>
+        <v>-0.01325</v>
       </c>
       <c r="F27" t="n">
         <v>-0.061</v>
@@ -1418,17 +1418,17 @@
         <v>-0.016</v>
       </c>
       <c r="H27" t="n">
-        <v>0.00073</v>
+        <v>0.00451</v>
       </c>
       <c r="I27" t="n">
-        <v>-0.00083</v>
+        <v>-0.00275</v>
       </c>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="n">
-        <v>1.05833</v>
+        <v>1.07</v>
       </c>
       <c r="L27" t="n">
-        <v>-15.23851</v>
+        <v>-17.14524</v>
       </c>
     </row>
     <row r="28">
@@ -1439,13 +1439,13 @@
         <v>13</v>
       </c>
       <c r="C28" t="n">
-        <v>0.26638</v>
+        <v>0.10944</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.13697</v>
+        <v>-0.13975</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.05527</v>
+        <v>-0.04613</v>
       </c>
       <c r="F28" t="n">
         <v>-0.135</v>
@@ -1454,17 +1454,17 @@
         <v>-0.058</v>
       </c>
       <c r="H28" t="n">
-        <v>0.00197</v>
+        <v>0.00475</v>
       </c>
       <c r="I28" t="n">
-        <v>-0.00273</v>
+        <v>-0.01187</v>
       </c>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="n">
-        <v>1.05191</v>
+        <v>1.06092</v>
       </c>
       <c r="L28" t="n">
-        <v>-15.27675</v>
+        <v>-17.11915</v>
       </c>
     </row>
     <row r="29">
@@ -1475,13 +1475,13 @@
         <v>14</v>
       </c>
       <c r="C29" t="n">
-        <v>0.26638</v>
+        <v>0.10944</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.14461</v>
+        <v>-0.15377</v>
       </c>
       <c r="E29" t="n">
-        <v>-0.05079</v>
+        <v>-0.04841</v>
       </c>
       <c r="F29" t="n">
         <v>-0.149</v>
@@ -1490,17 +1490,17 @@
         <v>-0.05</v>
       </c>
       <c r="H29" t="n">
-        <v>-0.00439</v>
+        <v>0.00477</v>
       </c>
       <c r="I29" t="n">
-        <v>0.00079</v>
+        <v>-0.00159</v>
       </c>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="n">
-        <v>1.02585</v>
+        <v>1.01648</v>
       </c>
       <c r="L29" t="n">
-        <v>-16.02996</v>
+        <v>-17.67622</v>
       </c>
     </row>
     <row r="30">
@@ -1511,19 +1511,19 @@
         <v>1</v>
       </c>
       <c r="C30" t="n">
-        <v>0.03385</v>
+        <v>0.00098</v>
       </c>
       <c r="D30" t="n">
-        <v>2.32373</v>
+        <v>2.35104</v>
       </c>
       <c r="E30" t="n">
-        <v>-0.15138</v>
+        <v>-0.52886</v>
       </c>
       <c r="F30" t="n">
         <v>2.324</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.14566</v>
+        <v>-0.53059</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
@@ -1533,7 +1533,7 @@
       </c>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="n">
-        <v>1.06</v>
+        <v>1</v>
       </c>
       <c r="L30" t="n">
         <v>-0</v>
@@ -1547,32 +1547,32 @@
         <v>2</v>
       </c>
       <c r="C31" t="n">
-        <v>0.03385</v>
+        <v>0.00098</v>
       </c>
       <c r="D31" t="n">
-        <v>0.18309</v>
+        <v>0.18301</v>
       </c>
       <c r="E31" t="n">
-        <v>0.35925</v>
+        <v>0.30997</v>
       </c>
       <c r="F31" t="n">
         <v>0.183</v>
       </c>
       <c r="G31" t="n">
-        <v>0.32852</v>
+        <v>0.20774</v>
       </c>
       <c r="H31" t="n">
-        <v>-9.000000000000001e-05</v>
+        <v>-1e-05</v>
       </c>
       <c r="I31" t="n">
         <v>0</v>
       </c>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="n">
-        <v>1.045</v>
+        <v>1</v>
       </c>
       <c r="L31" t="n">
-        <v>-4.99269</v>
+        <v>-5.8575</v>
       </c>
     </row>
     <row r="32">
@@ -1583,32 +1583,32 @@
         <v>3</v>
       </c>
       <c r="C32" t="n">
-        <v>0.03385</v>
+        <v>0.00098</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.94199</v>
+        <v>-0.94192</v>
       </c>
       <c r="E32" t="n">
-        <v>0.09429999999999999</v>
+        <v>0.40487</v>
       </c>
       <c r="F32" t="n">
         <v>-0.9419999999999999</v>
       </c>
       <c r="G32" t="n">
-        <v>0.09772</v>
+        <v>0.36428</v>
       </c>
       <c r="H32" t="n">
-        <v>-1e-05</v>
+        <v>-8.000000000000001e-05</v>
       </c>
       <c r="I32" t="n">
         <v>0</v>
       </c>
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="n">
-        <v>1.01</v>
+        <v>1</v>
       </c>
       <c r="L32" t="n">
-        <v>-12.76809</v>
+        <v>-14.69448</v>
       </c>
     </row>
     <row r="33">
@@ -1619,13 +1619,13 @@
         <v>4</v>
       </c>
       <c r="C33" t="n">
-        <v>0.03385</v>
+        <v>0.00098</v>
       </c>
       <c r="D33" t="n">
-        <v>-0.47746</v>
+        <v>-0.4777</v>
       </c>
       <c r="E33" t="n">
-        <v>0.039</v>
+        <v>0.03927</v>
       </c>
       <c r="F33" t="n">
         <v>-0.478</v>
@@ -1634,17 +1634,17 @@
         <v>0.039</v>
       </c>
       <c r="H33" t="n">
-        <v>-0.00054</v>
+        <v>-0.0003</v>
       </c>
       <c r="I33" t="n">
-        <v>-0</v>
+        <v>-0.00027</v>
       </c>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="n">
-        <v>1.01038</v>
+        <v>0.98154</v>
       </c>
       <c r="L33" t="n">
-        <v>-10.20464</v>
+        <v>-11.69663</v>
       </c>
     </row>
     <row r="34">
@@ -1655,13 +1655,13 @@
         <v>5</v>
       </c>
       <c r="C34" t="n">
-        <v>0.03385</v>
+        <v>0.00098</v>
       </c>
       <c r="D34" t="n">
         <v>-0.07562000000000001</v>
       </c>
       <c r="E34" t="n">
-        <v>-0.0156</v>
+        <v>-0.01502</v>
       </c>
       <c r="F34" t="n">
         <v>-0.076</v>
@@ -1673,14 +1673,14 @@
         <v>-0.00038</v>
       </c>
       <c r="I34" t="n">
-        <v>-0.0004</v>
+        <v>-0.00098</v>
       </c>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="n">
-        <v>1.01501</v>
+        <v>0.98452</v>
       </c>
       <c r="L34" t="n">
-        <v>-8.741440000000001</v>
+        <v>-10.17354</v>
       </c>
     </row>
     <row r="35">
@@ -1691,32 +1691,32 @@
         <v>6</v>
       </c>
       <c r="C35" t="n">
-        <v>0.03385</v>
+        <v>0.00098</v>
       </c>
       <c r="D35" t="n">
-        <v>-0.11213</v>
+        <v>-0.11196</v>
       </c>
       <c r="E35" t="n">
-        <v>0.16704</v>
+        <v>0.5114</v>
       </c>
       <c r="F35" t="n">
         <v>-0.112</v>
       </c>
       <c r="G35" t="n">
-        <v>0.165</v>
+        <v>0.51136</v>
       </c>
       <c r="H35" t="n">
-        <v>0.00013</v>
+        <v>-4e-05</v>
       </c>
       <c r="I35" t="n">
-        <v>-0.00204</v>
+        <v>-4e-05</v>
       </c>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="n">
-        <v>1.07154</v>
+        <v>1.08913</v>
       </c>
       <c r="L35" t="n">
-        <v>-14.43076</v>
+        <v>-16.32989</v>
       </c>
     </row>
     <row r="36">
@@ -1727,13 +1727,13 @@
         <v>7</v>
       </c>
       <c r="C36" t="n">
-        <v>0.03385</v>
+        <v>0.00098</v>
       </c>
       <c r="D36" t="n">
-        <v>0.00039</v>
+        <v>2e-05</v>
       </c>
       <c r="E36" t="n">
-        <v>-0.00032</v>
+        <v>0</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
@@ -1742,17 +1742,17 @@
         <v>0</v>
       </c>
       <c r="H36" t="n">
-        <v>-0.00039</v>
+        <v>-2e-05</v>
       </c>
       <c r="I36" t="n">
-        <v>0.00032</v>
+        <v>-0</v>
       </c>
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="n">
-        <v>1.02811</v>
+        <v>1</v>
       </c>
       <c r="L36" t="n">
-        <v>-13.23752</v>
+        <v>-14.70983</v>
       </c>
     </row>
     <row r="37">
@@ -1763,32 +1763,32 @@
         <v>8</v>
       </c>
       <c r="C37" t="n">
-        <v>0.03385</v>
+        <v>0.00098</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="E37" t="n">
-        <v>-0.03157</v>
+        <v>-0.13713</v>
       </c>
       <c r="F37" t="n">
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.06</v>
+        <v>-0.13757</v>
       </c>
       <c r="H37" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="I37" t="n">
-        <v>-0.02843</v>
+        <v>-0.00044</v>
       </c>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="n">
-        <v>1.01778</v>
+        <v>0.97528</v>
       </c>
       <c r="L37" t="n">
-        <v>-13.23752</v>
+        <v>-14.70983</v>
       </c>
     </row>
     <row r="38">
@@ -1799,13 +1799,13 @@
         <v>9</v>
       </c>
       <c r="C38" t="n">
-        <v>0.03385</v>
+        <v>0.00098</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.29567</v>
+        <v>-0.295</v>
       </c>
       <c r="E38" t="n">
-        <v>-0.16637</v>
+        <v>-0.16598</v>
       </c>
       <c r="F38" t="n">
         <v>-0.295</v>
@@ -1814,17 +1814,17 @@
         <v>-0.166</v>
       </c>
       <c r="H38" t="n">
-        <v>0.00067</v>
+        <v>-0</v>
       </c>
       <c r="I38" t="n">
-        <v>0.00037</v>
+        <v>-2e-05</v>
       </c>
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="n">
-        <v>1.0331</v>
+        <v>1.01464</v>
       </c>
       <c r="L38" t="n">
-        <v>-14.83244</v>
+        <v>-16.2772</v>
       </c>
     </row>
     <row r="39">
@@ -1835,13 +1835,13 @@
         <v>10</v>
       </c>
       <c r="C39" t="n">
-        <v>0.03385</v>
+        <v>0.00098</v>
       </c>
       <c r="D39" t="n">
-        <v>-0.08978999999999999</v>
+        <v>-0.09001000000000001</v>
       </c>
       <c r="E39" t="n">
-        <v>-0.05803</v>
+        <v>-0.058</v>
       </c>
       <c r="F39" t="n">
         <v>-0.09</v>
@@ -1850,17 +1850,17 @@
         <v>-0.058</v>
       </c>
       <c r="H39" t="n">
-        <v>-0.00021</v>
+        <v>1e-05</v>
       </c>
       <c r="I39" t="n">
-        <v>3e-05</v>
+        <v>-0</v>
       </c>
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="n">
-        <v>1.03232</v>
+        <v>1.02013</v>
       </c>
       <c r="L39" t="n">
-        <v>-15.0425</v>
+        <v>-16.5561</v>
       </c>
     </row>
     <row r="40">
@@ -1871,13 +1871,13 @@
         <v>11</v>
       </c>
       <c r="C40" t="n">
-        <v>0.03385</v>
+        <v>0.00098</v>
       </c>
       <c r="D40" t="n">
-        <v>-0.03455</v>
+        <v>-0.035</v>
       </c>
       <c r="E40" t="n">
-        <v>-0.01813</v>
+        <v>-0.018</v>
       </c>
       <c r="F40" t="n">
         <v>-0.035</v>
@@ -1886,17 +1886,17 @@
         <v>-0.018</v>
       </c>
       <c r="H40" t="n">
-        <v>-0.00045</v>
+        <v>-0</v>
       </c>
       <c r="I40" t="n">
-        <v>0.00013</v>
+        <v>-0</v>
       </c>
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="n">
-        <v>1.04811</v>
+        <v>1.05051</v>
       </c>
       <c r="L40" t="n">
-        <v>-14.85345</v>
+        <v>-16.53917</v>
       </c>
     </row>
     <row r="41">
@@ -1907,13 +1907,13 @@
         <v>12</v>
       </c>
       <c r="C41" t="n">
-        <v>0.03385</v>
+        <v>0.00098</v>
       </c>
       <c r="D41" t="n">
-        <v>-0.06101</v>
+        <v>-0.061</v>
       </c>
       <c r="E41" t="n">
-        <v>-0.01597</v>
+        <v>-0.016</v>
       </c>
       <c r="F41" t="n">
         <v>-0.061</v>
@@ -1922,17 +1922,17 @@
         <v>-0.016</v>
       </c>
       <c r="H41" t="n">
-        <v>1e-05</v>
+        <v>-0</v>
       </c>
       <c r="I41" t="n">
-        <v>-3e-05</v>
+        <v>-0</v>
       </c>
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="n">
-        <v>1.0549</v>
+        <v>1.07</v>
       </c>
       <c r="L41" t="n">
-        <v>-15.27984</v>
+        <v>-17.14995</v>
       </c>
     </row>
     <row r="42">
@@ -1943,13 +1943,13 @@
         <v>13</v>
       </c>
       <c r="C42" t="n">
-        <v>0.03385</v>
+        <v>0.00098</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.13478</v>
+        <v>-0.13499</v>
       </c>
       <c r="E42" t="n">
-        <v>-0.05806</v>
+        <v>-0.05799</v>
       </c>
       <c r="F42" t="n">
         <v>-0.135</v>
@@ -1958,17 +1958,17 @@
         <v>-0.058</v>
       </c>
       <c r="H42" t="n">
-        <v>-0.00022</v>
+        <v>-1e-05</v>
       </c>
       <c r="I42" t="n">
-        <v>6e-05</v>
+        <v>-1e-05</v>
       </c>
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="n">
-        <v>1.04835</v>
+        <v>1.06092</v>
       </c>
       <c r="L42" t="n">
-        <v>-15.31667</v>
+        <v>-17.12381</v>
       </c>
     </row>
     <row r="43">
@@ -1979,13 +1979,13 @@
         <v>14</v>
       </c>
       <c r="C43" t="n">
-        <v>0.03385</v>
+        <v>0.00098</v>
       </c>
       <c r="D43" t="n">
-        <v>-0.14876</v>
+        <v>-0.14901</v>
       </c>
       <c r="E43" t="n">
-        <v>-0.05008</v>
+        <v>-0.04999</v>
       </c>
       <c r="F43" t="n">
         <v>-0.149</v>
@@ -1994,1025 +1994,17 @@
         <v>-0.05</v>
       </c>
       <c r="H43" t="n">
-        <v>-0.00024</v>
+        <v>1e-05</v>
       </c>
       <c r="I43" t="n">
-        <v>8.000000000000001e-05</v>
+        <v>-1e-05</v>
       </c>
       <c r="J43" t="inlineStr"/>
       <c r="K43" t="n">
-        <v>1.02151</v>
+        <v>1.01647</v>
       </c>
       <c r="L43" t="n">
-        <v>-16.06782</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="n">
-        <v>4</v>
-      </c>
-      <c r="B44" t="n">
-        <v>1</v>
-      </c>
-      <c r="C44" t="n">
-        <v>0.02811</v>
-      </c>
-      <c r="D44" t="n">
-        <v>2.3261</v>
-      </c>
-      <c r="E44" t="n">
-        <v>-0.14526</v>
-      </c>
-      <c r="F44" t="n">
-        <v>2.324</v>
-      </c>
-      <c r="G44" t="n">
-        <v>-0.15138</v>
-      </c>
-      <c r="H44" t="n">
-        <v>0</v>
-      </c>
-      <c r="I44" t="n">
-        <v>0</v>
-      </c>
-      <c r="J44" t="inlineStr"/>
-      <c r="K44" t="n">
-        <v>1.06</v>
-      </c>
-      <c r="L44" t="n">
-        <v>-0</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n">
-        <v>4</v>
-      </c>
-      <c r="B45" t="n">
-        <v>2</v>
-      </c>
-      <c r="C45" t="n">
-        <v>0.02811</v>
-      </c>
-      <c r="D45" t="n">
-        <v>0.18301</v>
-      </c>
-      <c r="E45" t="n">
-        <v>0.37815</v>
-      </c>
-      <c r="F45" t="n">
-        <v>0.183</v>
-      </c>
-      <c r="G45" t="n">
-        <v>0.35925</v>
-      </c>
-      <c r="H45" t="n">
-        <v>-1e-05</v>
-      </c>
-      <c r="I45" t="n">
-        <v>-0.0189</v>
-      </c>
-      <c r="J45" t="inlineStr"/>
-      <c r="K45" t="n">
-        <v>1.04432</v>
-      </c>
-      <c r="L45" t="n">
-        <v>-4.98379</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>4</v>
-      </c>
-      <c r="B46" t="n">
-        <v>3</v>
-      </c>
-      <c r="C46" t="n">
-        <v>0.02811</v>
-      </c>
-      <c r="D46" t="n">
-        <v>-0.9419999999999999</v>
-      </c>
-      <c r="E46" t="n">
-        <v>0.10446</v>
-      </c>
-      <c r="F46" t="n">
-        <v>-0.9419999999999999</v>
-      </c>
-      <c r="G46" t="n">
-        <v>0.09429999999999999</v>
-      </c>
-      <c r="H46" t="n">
-        <v>-0</v>
-      </c>
-      <c r="I46" t="n">
-        <v>0</v>
-      </c>
-      <c r="J46" t="inlineStr"/>
-      <c r="K46" t="n">
-        <v>1.01</v>
-      </c>
-      <c r="L46" t="n">
-        <v>-12.77617</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>4</v>
-      </c>
-      <c r="B47" t="n">
-        <v>4</v>
-      </c>
-      <c r="C47" t="n">
-        <v>0.02811</v>
-      </c>
-      <c r="D47" t="n">
-        <v>-0.47801</v>
-      </c>
-      <c r="E47" t="n">
-        <v>0.039</v>
-      </c>
-      <c r="F47" t="n">
-        <v>-0.478</v>
-      </c>
-      <c r="G47" t="n">
-        <v>0.039</v>
-      </c>
-      <c r="H47" t="n">
-        <v>1e-05</v>
-      </c>
-      <c r="I47" t="n">
-        <v>-0</v>
-      </c>
-      <c r="J47" t="inlineStr"/>
-      <c r="K47" t="n">
-        <v>1.00997</v>
-      </c>
-      <c r="L47" t="n">
-        <v>-10.20503</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>4</v>
-      </c>
-      <c r="B48" t="n">
-        <v>5</v>
-      </c>
-      <c r="C48" t="n">
-        <v>0.02811</v>
-      </c>
-      <c r="D48" t="n">
-        <v>-0.07600999999999999</v>
-      </c>
-      <c r="E48" t="n">
-        <v>-0.016</v>
-      </c>
-      <c r="F48" t="n">
-        <v>-0.076</v>
-      </c>
-      <c r="G48" t="n">
-        <v>-0.016</v>
-      </c>
-      <c r="H48" t="n">
-        <v>1e-05</v>
-      </c>
-      <c r="I48" t="n">
-        <v>-0</v>
-      </c>
-      <c r="J48" t="inlineStr"/>
-      <c r="K48" t="n">
-        <v>1.01461</v>
-      </c>
-      <c r="L48" t="n">
-        <v>-8.740729999999999</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n">
-        <v>4</v>
-      </c>
-      <c r="B49" t="n">
-        <v>6</v>
-      </c>
-      <c r="C49" t="n">
-        <v>0.02811</v>
-      </c>
-      <c r="D49" t="n">
-        <v>-0.112</v>
-      </c>
-      <c r="E49" t="n">
-        <v>0.16501</v>
-      </c>
-      <c r="F49" t="n">
-        <v>-0.112</v>
-      </c>
-      <c r="G49" t="n">
-        <v>0.165</v>
-      </c>
-      <c r="H49" t="n">
-        <v>-0</v>
-      </c>
-      <c r="I49" t="n">
-        <v>-1e-05</v>
-      </c>
-      <c r="J49" t="inlineStr"/>
-      <c r="K49" t="n">
-        <v>1.07108</v>
-      </c>
-      <c r="L49" t="n">
-        <v>-14.43515</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n">
-        <v>4</v>
-      </c>
-      <c r="B50" t="n">
-        <v>7</v>
-      </c>
-      <c r="C50" t="n">
-        <v>0.02811</v>
-      </c>
-      <c r="D50" t="n">
-        <v>-0</v>
-      </c>
-      <c r="E50" t="n">
-        <v>-0</v>
-      </c>
-      <c r="F50" t="n">
-        <v>0</v>
-      </c>
-      <c r="G50" t="n">
-        <v>0</v>
-      </c>
-      <c r="H50" t="n">
-        <v>0</v>
-      </c>
-      <c r="I50" t="n">
-        <v>0</v>
-      </c>
-      <c r="J50" t="inlineStr"/>
-      <c r="K50" t="n">
-        <v>1.02763</v>
-      </c>
-      <c r="L50" t="n">
-        <v>-13.24057</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="n">
-        <v>4</v>
-      </c>
-      <c r="B51" t="n">
-        <v>8</v>
-      </c>
-      <c r="C51" t="n">
-        <v>0.02811</v>
-      </c>
-      <c r="D51" t="n">
-        <v>-0</v>
-      </c>
-      <c r="E51" t="n">
-        <v>-0.0597</v>
-      </c>
-      <c r="F51" t="n">
-        <v>0</v>
-      </c>
-      <c r="G51" t="n">
-        <v>-0.06</v>
-      </c>
-      <c r="H51" t="n">
-        <v>0</v>
-      </c>
-      <c r="I51" t="n">
-        <v>-0.0003</v>
-      </c>
-      <c r="J51" t="inlineStr"/>
-      <c r="K51" t="n">
-        <v>1.01724</v>
-      </c>
-      <c r="L51" t="n">
-        <v>-13.24057</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>4</v>
-      </c>
-      <c r="B52" t="n">
-        <v>9</v>
-      </c>
-      <c r="C52" t="n">
-        <v>0.02811</v>
-      </c>
-      <c r="D52" t="n">
-        <v>-0.295</v>
-      </c>
-      <c r="E52" t="n">
-        <v>-0.16599</v>
-      </c>
-      <c r="F52" t="n">
-        <v>-0.295</v>
-      </c>
-      <c r="G52" t="n">
-        <v>-0.166</v>
-      </c>
-      <c r="H52" t="n">
-        <v>-0</v>
-      </c>
-      <c r="I52" t="n">
-        <v>-1e-05</v>
-      </c>
-      <c r="J52" t="inlineStr"/>
-      <c r="K52" t="n">
-        <v>1.03261</v>
-      </c>
-      <c r="L52" t="n">
-        <v>-14.83703</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>4</v>
-      </c>
-      <c r="B53" t="n">
-        <v>10</v>
-      </c>
-      <c r="C53" t="n">
-        <v>0.02811</v>
-      </c>
-      <c r="D53" t="n">
-        <v>-0.08999</v>
-      </c>
-      <c r="E53" t="n">
-        <v>-0.058</v>
-      </c>
-      <c r="F53" t="n">
-        <v>-0.09</v>
-      </c>
-      <c r="G53" t="n">
-        <v>-0.058</v>
-      </c>
-      <c r="H53" t="n">
-        <v>-1e-05</v>
-      </c>
-      <c r="I53" t="n">
-        <v>0</v>
-      </c>
-      <c r="J53" t="inlineStr"/>
-      <c r="K53" t="n">
-        <v>1.03184</v>
-      </c>
-      <c r="L53" t="n">
-        <v>-15.04734</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>4</v>
-      </c>
-      <c r="B54" t="n">
-        <v>11</v>
-      </c>
-      <c r="C54" t="n">
-        <v>0.02811</v>
-      </c>
-      <c r="D54" t="n">
-        <v>-0.035</v>
-      </c>
-      <c r="E54" t="n">
-        <v>-0.018</v>
-      </c>
-      <c r="F54" t="n">
-        <v>-0.035</v>
-      </c>
-      <c r="G54" t="n">
-        <v>-0.018</v>
-      </c>
-      <c r="H54" t="n">
-        <v>-0</v>
-      </c>
-      <c r="I54" t="n">
-        <v>0</v>
-      </c>
-      <c r="J54" t="inlineStr"/>
-      <c r="K54" t="n">
-        <v>1.04764</v>
-      </c>
-      <c r="L54" t="n">
-        <v>-14.85818</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>4</v>
-      </c>
-      <c r="B55" t="n">
-        <v>12</v>
-      </c>
-      <c r="C55" t="n">
-        <v>0.02811</v>
-      </c>
-      <c r="D55" t="n">
-        <v>-0.061</v>
-      </c>
-      <c r="E55" t="n">
-        <v>-0.016</v>
-      </c>
-      <c r="F55" t="n">
-        <v>-0.061</v>
-      </c>
-      <c r="G55" t="n">
-        <v>-0.016</v>
-      </c>
-      <c r="H55" t="n">
-        <v>-0</v>
-      </c>
-      <c r="I55" t="n">
-        <v>0</v>
-      </c>
-      <c r="J55" t="inlineStr"/>
-      <c r="K55" t="n">
-        <v>1.05443</v>
-      </c>
-      <c r="L55" t="n">
-        <v>-15.28501</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>4</v>
-      </c>
-      <c r="B56" t="n">
-        <v>13</v>
-      </c>
-      <c r="C56" t="n">
-        <v>0.02811</v>
-      </c>
-      <c r="D56" t="n">
-        <v>-0.135</v>
-      </c>
-      <c r="E56" t="n">
-        <v>-0.058</v>
-      </c>
-      <c r="F56" t="n">
-        <v>-0.135</v>
-      </c>
-      <c r="G56" t="n">
-        <v>-0.058</v>
-      </c>
-      <c r="H56" t="n">
-        <v>-0</v>
-      </c>
-      <c r="I56" t="n">
-        <v>0</v>
-      </c>
-      <c r="J56" t="inlineStr"/>
-      <c r="K56" t="n">
-        <v>1.04788</v>
-      </c>
-      <c r="L56" t="n">
-        <v>-15.32186</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>4</v>
-      </c>
-      <c r="B57" t="n">
-        <v>14</v>
-      </c>
-      <c r="C57" t="n">
-        <v>0.02811</v>
-      </c>
-      <c r="D57" t="n">
-        <v>-0.14899</v>
-      </c>
-      <c r="E57" t="n">
-        <v>-0.05</v>
-      </c>
-      <c r="F57" t="n">
-        <v>-0.149</v>
-      </c>
-      <c r="G57" t="n">
-        <v>-0.05</v>
-      </c>
-      <c r="H57" t="n">
-        <v>-1e-05</v>
-      </c>
-      <c r="I57" t="n">
-        <v>0</v>
-      </c>
-      <c r="J57" t="inlineStr"/>
-      <c r="K57" t="n">
-        <v>1.02102</v>
-      </c>
-      <c r="L57" t="n">
-        <v>-16.07371</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>5</v>
-      </c>
-      <c r="B58" t="n">
-        <v>1</v>
-      </c>
-      <c r="C58" t="n">
-        <v>0.02763</v>
-      </c>
-      <c r="D58" t="n">
-        <v>2.32613</v>
-      </c>
-      <c r="E58" t="n">
-        <v>-0.13154</v>
-      </c>
-      <c r="F58" t="n">
-        <v>2.324</v>
-      </c>
-      <c r="G58" t="n">
-        <v>-0.14526</v>
-      </c>
-      <c r="H58" t="n">
-        <v>0</v>
-      </c>
-      <c r="I58" t="n">
-        <v>0</v>
-      </c>
-      <c r="J58" t="inlineStr"/>
-      <c r="K58" t="n">
-        <v>1.06</v>
-      </c>
-      <c r="L58" t="n">
-        <v>-0</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>5</v>
-      </c>
-      <c r="B59" t="n">
-        <v>2</v>
-      </c>
-      <c r="C59" t="n">
-        <v>0.02763</v>
-      </c>
-      <c r="D59" t="n">
-        <v>0.183</v>
-      </c>
-      <c r="E59" t="n">
-        <v>0.35927</v>
-      </c>
-      <c r="F59" t="n">
-        <v>0.183</v>
-      </c>
-      <c r="G59" t="n">
-        <v>0.373</v>
-      </c>
-      <c r="H59" t="n">
-        <v>0</v>
-      </c>
-      <c r="I59" t="n">
-        <v>0.01373</v>
-      </c>
-      <c r="J59" t="inlineStr"/>
-      <c r="K59" t="n">
-        <v>1.04481</v>
-      </c>
-      <c r="L59" t="n">
-        <v>-4.99027</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>5</v>
-      </c>
-      <c r="B60" t="n">
-        <v>3</v>
-      </c>
-      <c r="C60" t="n">
-        <v>0.02763</v>
-      </c>
-      <c r="D60" t="n">
-        <v>-0.9419999999999999</v>
-      </c>
-      <c r="E60" t="n">
-        <v>0.11048</v>
-      </c>
-      <c r="F60" t="n">
-        <v>-0.9419999999999999</v>
-      </c>
-      <c r="G60" t="n">
-        <v>0.10446</v>
-      </c>
-      <c r="H60" t="n">
-        <v>-0</v>
-      </c>
-      <c r="I60" t="n">
-        <v>0</v>
-      </c>
-      <c r="J60" t="inlineStr"/>
-      <c r="K60" t="n">
-        <v>1.01</v>
-      </c>
-      <c r="L60" t="n">
-        <v>-12.77052</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>5</v>
-      </c>
-      <c r="B61" t="n">
-        <v>4</v>
-      </c>
-      <c r="C61" t="n">
-        <v>0.02763</v>
-      </c>
-      <c r="D61" t="n">
-        <v>-0.478</v>
-      </c>
-      <c r="E61" t="n">
-        <v>0.039</v>
-      </c>
-      <c r="F61" t="n">
-        <v>-0.478</v>
-      </c>
-      <c r="G61" t="n">
-        <v>0.039</v>
-      </c>
-      <c r="H61" t="n">
-        <v>-0</v>
-      </c>
-      <c r="I61" t="n">
-        <v>0</v>
-      </c>
-      <c r="J61" t="inlineStr"/>
-      <c r="K61" t="n">
-        <v>1.01025</v>
-      </c>
-      <c r="L61" t="n">
-        <v>-10.20466</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="n">
-        <v>5</v>
-      </c>
-      <c r="B62" t="n">
-        <v>5</v>
-      </c>
-      <c r="C62" t="n">
-        <v>0.02763</v>
-      </c>
-      <c r="D62" t="n">
-        <v>-0.076</v>
-      </c>
-      <c r="E62" t="n">
-        <v>-0.016</v>
-      </c>
-      <c r="F62" t="n">
-        <v>-0.076</v>
-      </c>
-      <c r="G62" t="n">
-        <v>-0.016</v>
-      </c>
-      <c r="H62" t="n">
-        <v>-0</v>
-      </c>
-      <c r="I62" t="n">
-        <v>0</v>
-      </c>
-      <c r="J62" t="inlineStr"/>
-      <c r="K62" t="n">
-        <v>1.01489</v>
-      </c>
-      <c r="L62" t="n">
-        <v>-8.74119</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="n">
-        <v>5</v>
-      </c>
-      <c r="B63" t="n">
-        <v>6</v>
-      </c>
-      <c r="C63" t="n">
-        <v>0.02763</v>
-      </c>
-      <c r="D63" t="n">
-        <v>-0.112</v>
-      </c>
-      <c r="E63" t="n">
-        <v>0.165</v>
-      </c>
-      <c r="F63" t="n">
-        <v>-0.112</v>
-      </c>
-      <c r="G63" t="n">
-        <v>0.165</v>
-      </c>
-      <c r="H63" t="n">
-        <v>-0</v>
-      </c>
-      <c r="I63" t="n">
-        <v>-0</v>
-      </c>
-      <c r="J63" t="inlineStr"/>
-      <c r="K63" t="n">
-        <v>1.07138</v>
-      </c>
-      <c r="L63" t="n">
-        <v>-14.43237</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="n">
-        <v>5</v>
-      </c>
-      <c r="B64" t="n">
-        <v>7</v>
-      </c>
-      <c r="C64" t="n">
-        <v>0.02763</v>
-      </c>
-      <c r="D64" t="n">
-        <v>-0</v>
-      </c>
-      <c r="E64" t="n">
-        <v>-0</v>
-      </c>
-      <c r="F64" t="n">
-        <v>0</v>
-      </c>
-      <c r="G64" t="n">
-        <v>0</v>
-      </c>
-      <c r="H64" t="n">
-        <v>0</v>
-      </c>
-      <c r="I64" t="n">
-        <v>0</v>
-      </c>
-      <c r="J64" t="inlineStr"/>
-      <c r="K64" t="n">
-        <v>1.02793</v>
-      </c>
-      <c r="L64" t="n">
-        <v>-13.23845</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="n">
-        <v>5</v>
-      </c>
-      <c r="B65" t="n">
-        <v>8</v>
-      </c>
-      <c r="C65" t="n">
-        <v>0.02763</v>
-      </c>
-      <c r="D65" t="n">
-        <v>0</v>
-      </c>
-      <c r="E65" t="n">
-        <v>-0.06</v>
-      </c>
-      <c r="F65" t="n">
-        <v>0</v>
-      </c>
-      <c r="G65" t="n">
-        <v>-0.06</v>
-      </c>
-      <c r="H65" t="n">
-        <v>-0</v>
-      </c>
-      <c r="I65" t="n">
-        <v>-0</v>
-      </c>
-      <c r="J65" t="inlineStr"/>
-      <c r="K65" t="n">
-        <v>1.01754</v>
-      </c>
-      <c r="L65" t="n">
-        <v>-13.23845</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="n">
-        <v>5</v>
-      </c>
-      <c r="B66" t="n">
-        <v>9</v>
-      </c>
-      <c r="C66" t="n">
-        <v>0.02763</v>
-      </c>
-      <c r="D66" t="n">
-        <v>-0.295</v>
-      </c>
-      <c r="E66" t="n">
-        <v>-0.166</v>
-      </c>
-      <c r="F66" t="n">
-        <v>-0.295</v>
-      </c>
-      <c r="G66" t="n">
-        <v>-0.166</v>
-      </c>
-      <c r="H66" t="n">
-        <v>-0</v>
-      </c>
-      <c r="I66" t="n">
-        <v>-0</v>
-      </c>
-      <c r="J66" t="inlineStr"/>
-      <c r="K66" t="n">
-        <v>1.03292</v>
-      </c>
-      <c r="L66" t="n">
-        <v>-14.83395</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="n">
-        <v>5</v>
-      </c>
-      <c r="B67" t="n">
-        <v>10</v>
-      </c>
-      <c r="C67" t="n">
-        <v>0.02763</v>
-      </c>
-      <c r="D67" t="n">
-        <v>-0.09</v>
-      </c>
-      <c r="E67" t="n">
-        <v>-0.058</v>
-      </c>
-      <c r="F67" t="n">
-        <v>-0.09</v>
-      </c>
-      <c r="G67" t="n">
-        <v>-0.058</v>
-      </c>
-      <c r="H67" t="n">
-        <v>-0</v>
-      </c>
-      <c r="I67" t="n">
-        <v>-0</v>
-      </c>
-      <c r="J67" t="inlineStr"/>
-      <c r="K67" t="n">
-        <v>1.03215</v>
-      </c>
-      <c r="L67" t="n">
-        <v>-15.04415</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="n">
-        <v>5</v>
-      </c>
-      <c r="B68" t="n">
-        <v>11</v>
-      </c>
-      <c r="C68" t="n">
-        <v>0.02763</v>
-      </c>
-      <c r="D68" t="n">
-        <v>-0.035</v>
-      </c>
-      <c r="E68" t="n">
-        <v>-0.018</v>
-      </c>
-      <c r="F68" t="n">
-        <v>-0.035</v>
-      </c>
-      <c r="G68" t="n">
-        <v>-0.018</v>
-      </c>
-      <c r="H68" t="n">
-        <v>-0</v>
-      </c>
-      <c r="I68" t="n">
-        <v>0</v>
-      </c>
-      <c r="J68" t="inlineStr"/>
-      <c r="K68" t="n">
-        <v>1.04795</v>
-      </c>
-      <c r="L68" t="n">
-        <v>-14.85513</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="n">
-        <v>5</v>
-      </c>
-      <c r="B69" t="n">
-        <v>12</v>
-      </c>
-      <c r="C69" t="n">
-        <v>0.02763</v>
-      </c>
-      <c r="D69" t="n">
-        <v>-0.061</v>
-      </c>
-      <c r="E69" t="n">
-        <v>-0.016</v>
-      </c>
-      <c r="F69" t="n">
-        <v>-0.061</v>
-      </c>
-      <c r="G69" t="n">
-        <v>-0.016</v>
-      </c>
-      <c r="H69" t="n">
-        <v>-0</v>
-      </c>
-      <c r="I69" t="n">
-        <v>0</v>
-      </c>
-      <c r="J69" t="inlineStr"/>
-      <c r="K69" t="n">
-        <v>1.05474</v>
-      </c>
-      <c r="L69" t="n">
-        <v>-15.28174</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="n">
-        <v>5</v>
-      </c>
-      <c r="B70" t="n">
-        <v>13</v>
-      </c>
-      <c r="C70" t="n">
-        <v>0.02763</v>
-      </c>
-      <c r="D70" t="n">
-        <v>-0.135</v>
-      </c>
-      <c r="E70" t="n">
-        <v>-0.058</v>
-      </c>
-      <c r="F70" t="n">
-        <v>-0.135</v>
-      </c>
-      <c r="G70" t="n">
-        <v>-0.058</v>
-      </c>
-      <c r="H70" t="n">
-        <v>-0</v>
-      </c>
-      <c r="I70" t="n">
-        <v>0</v>
-      </c>
-      <c r="J70" t="inlineStr"/>
-      <c r="K70" t="n">
-        <v>1.04819</v>
-      </c>
-      <c r="L70" t="n">
-        <v>-15.31855</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="n">
-        <v>5</v>
-      </c>
-      <c r="B71" t="n">
-        <v>14</v>
-      </c>
-      <c r="C71" t="n">
-        <v>0.02763</v>
-      </c>
-      <c r="D71" t="n">
-        <v>-0.149</v>
-      </c>
-      <c r="E71" t="n">
-        <v>-0.05</v>
-      </c>
-      <c r="F71" t="n">
-        <v>-0.149</v>
-      </c>
-      <c r="G71" t="n">
-        <v>-0.05</v>
-      </c>
-      <c r="H71" t="n">
-        <v>-0</v>
-      </c>
-      <c r="I71" t="n">
-        <v>0</v>
-      </c>
-      <c r="J71" t="inlineStr"/>
-      <c r="K71" t="n">
-        <v>1.02134</v>
-      </c>
-      <c r="L71" t="n">
-        <v>-16.06991</v>
+        <v>-17.68071</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionei um novo código de controle e fiz diversos ajustes no código de tap
</commit_message>
<xml_diff>
--- a/relatorio_iteracoes_NR.xlsx
+++ b/relatorio_iteracoes_NR.xlsx
@@ -503,19 +503,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9419999999999999</v>
+        <v>1.23434</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>2.33115</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.051</v>
+        <v>-0.16914</v>
       </c>
       <c r="F2" t="n">
         <v>2.324</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.169</v>
+        <v>-0.163</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -525,10 +525,10 @@
       </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>1.06</v>
       </c>
       <c r="L2" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -539,32 +539,32 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9419999999999999</v>
+        <v>1.23434</v>
       </c>
       <c r="D3" t="n">
-        <v>-0</v>
+        <v>0.1701</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.08260000000000001</v>
+        <v>0.3167</v>
       </c>
       <c r="F3" t="n">
         <v>0.183</v>
       </c>
       <c r="G3" t="n">
-        <v>0.297</v>
+        <v>0.3178</v>
       </c>
       <c r="H3" t="n">
-        <v>0.183</v>
+        <v>0.0129</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
       </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="n">
-        <v>1</v>
+        <v>1.045</v>
       </c>
       <c r="L3" t="n">
-        <v>-5.44124</v>
+        <v>-4.97689</v>
       </c>
     </row>
     <row r="4">
@@ -575,32 +575,32 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9419999999999999</v>
+        <v>1.23434</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>-1.01461</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.0283</v>
+        <v>0.09599000000000001</v>
       </c>
       <c r="F4" t="n">
         <v>-0.9419999999999999</v>
       </c>
       <c r="G4" t="n">
-        <v>0.044</v>
+        <v>0.0667</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.9419999999999999</v>
+        <v>0.07260999999999999</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
       </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="n">
-        <v>1</v>
+        <v>1.01</v>
       </c>
       <c r="L4" t="n">
-        <v>-13.97862</v>
+        <v>-12.7091</v>
       </c>
     </row>
     <row r="5">
@@ -611,13 +611,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9419999999999999</v>
+        <v>1.23434</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>-0.27914</v>
       </c>
       <c r="E5" t="n">
-        <v>0.14595</v>
+        <v>0.2241</v>
       </c>
       <c r="F5" t="n">
         <v>-0.478</v>
@@ -626,17 +626,17 @@
         <v>0.039</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.478</v>
+        <v>-0.19886</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.10695</v>
+        <v>-0.1851</v>
       </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="n">
-        <v>0.98697</v>
+        <v>1.01928</v>
       </c>
       <c r="L5" t="n">
-        <v>-11.09221</v>
+        <v>-10.33022</v>
       </c>
     </row>
     <row r="6">
@@ -647,13 +647,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9419999999999999</v>
+        <v>1.23434</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>-0.2232</v>
       </c>
       <c r="E6" t="n">
-        <v>0.26873</v>
+        <v>0.05461</v>
       </c>
       <c r="F6" t="n">
         <v>-0.076</v>
@@ -662,17 +662,17 @@
         <v>-0.016</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.076</v>
+        <v>0.1472</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.28473</v>
+        <v>-0.07061000000000001</v>
       </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="n">
-        <v>0.99136</v>
+        <v>1.02056</v>
       </c>
       <c r="L6" t="n">
-        <v>-9.61924</v>
+        <v>-8.77496</v>
       </c>
     </row>
     <row r="7">
@@ -683,32 +683,32 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9419999999999999</v>
+        <v>1.23434</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.10682</v>
+        <v>-0.06979</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.5118200000000001</v>
+        <v>-0.03997</v>
       </c>
       <c r="F7" t="n">
         <v>-0.112</v>
       </c>
       <c r="G7" t="n">
-        <v>0.047</v>
+        <v>0.0418</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.00518</v>
+        <v>-0.04221</v>
       </c>
       <c r="I7" t="n">
-        <v>0.55882</v>
+        <v>0</v>
       </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="n">
-        <v>1.08854</v>
+        <v>1.07</v>
       </c>
       <c r="L7" t="n">
-        <v>-15.70933</v>
+        <v>-14.1594</v>
       </c>
     </row>
     <row r="8">
@@ -719,13 +719,13 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9419999999999999</v>
+        <v>1.23434</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>0.07603</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.10757</v>
+        <v>-1.23434</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -734,17 +734,17 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>-0.07603</v>
       </c>
       <c r="I8" t="n">
-        <v>0.10757</v>
+        <v>1.23434</v>
       </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="n">
-        <v>1</v>
+        <v>1.06855</v>
       </c>
       <c r="L8" t="n">
-        <v>-14.0804</v>
+        <v>-13.38866</v>
       </c>
     </row>
     <row r="9">
@@ -755,32 +755,32 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>0.9419999999999999</v>
+        <v>1.23434</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>0.55691</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.174</v>
+        <v>0.1668</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>0.174</v>
+        <v>0</v>
       </c>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="n">
-        <v>0.9664199999999999</v>
+        <v>1.09</v>
       </c>
       <c r="L9" t="n">
-        <v>-14.0804</v>
+        <v>-13.38866</v>
       </c>
     </row>
     <row r="10">
@@ -791,13 +791,13 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9419999999999999</v>
+        <v>1.23434</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>-0.39418</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.24752</v>
+        <v>0.50779</v>
       </c>
       <c r="F10" t="n">
         <v>-0.295</v>
@@ -806,17 +806,17 @@
         <v>-0.166</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.295</v>
+        <v>0.09918</v>
       </c>
       <c r="I10" t="n">
-        <v>0.08152</v>
+        <v>-0.67379</v>
       </c>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="n">
-        <v>1.01615</v>
+        <v>1.06084</v>
       </c>
       <c r="L10" t="n">
-        <v>-15.68773</v>
+        <v>-14.93733</v>
       </c>
     </row>
     <row r="11">
@@ -827,13 +827,13 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9419999999999999</v>
+        <v>1.23434</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>-0.03459</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>-0.08875</v>
       </c>
       <c r="F11" t="n">
         <v>-0.09</v>
@@ -842,17 +842,17 @@
         <v>-0.058</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.09</v>
+        <v>-0.05541</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.058</v>
+        <v>0.03075</v>
       </c>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="n">
-        <v>1.0211</v>
+        <v>1.05507</v>
       </c>
       <c r="L11" t="n">
-        <v>-15.9772</v>
+        <v>-15.08666</v>
       </c>
     </row>
     <row r="12">
@@ -863,13 +863,13 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9419999999999999</v>
+        <v>1.23434</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>-0.09344</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>0.01499</v>
       </c>
       <c r="F12" t="n">
         <v>-0.035</v>
@@ -878,17 +878,17 @@
         <v>-0.018</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.035</v>
+        <v>0.05844</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.018</v>
+        <v>-0.03299</v>
       </c>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="n">
-        <v>1.05056</v>
+        <v>1.05902</v>
       </c>
       <c r="L12" t="n">
-        <v>-15.95706</v>
+        <v>-14.75749</v>
       </c>
     </row>
     <row r="13">
@@ -899,13 +899,13 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>0.9419999999999999</v>
+        <v>1.23434</v>
       </c>
       <c r="D13" t="n">
-        <v>0.30072</v>
+        <v>-0.01259</v>
       </c>
       <c r="E13" t="n">
-        <v>0.40655</v>
+        <v>0.07683</v>
       </c>
       <c r="F13" t="n">
         <v>-0.061</v>
@@ -914,17 +914,17 @@
         <v>-0.016</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.36172</v>
+        <v>-0.04841</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.42255</v>
+        <v>-0.09283</v>
       </c>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="n">
-        <v>1.07</v>
+        <v>1.05578</v>
       </c>
       <c r="L13" t="n">
-        <v>-16.60005</v>
+        <v>-15.01521</v>
       </c>
     </row>
     <row r="14">
@@ -935,13 +935,13 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>0.9419999999999999</v>
+        <v>1.23434</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.17423</v>
+        <v>-0.17103</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.15764</v>
+        <v>-0.0946</v>
       </c>
       <c r="F14" t="n">
         <v>-0.135</v>
@@ -950,17 +950,17 @@
         <v>-0.058</v>
       </c>
       <c r="H14" t="n">
-        <v>0.03923</v>
+        <v>0.03603</v>
       </c>
       <c r="I14" t="n">
-        <v>0.09964000000000001</v>
+        <v>0.0366</v>
       </c>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="n">
-        <v>1.0614</v>
+        <v>1.05117</v>
       </c>
       <c r="L14" t="n">
-        <v>-16.58094</v>
+        <v>-15.10284</v>
       </c>
     </row>
     <row r="15">
@@ -971,13 +971,13 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>0.9419999999999999</v>
+        <v>1.23434</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>-0.14967</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>-0.05052</v>
       </c>
       <c r="F15" t="n">
         <v>-0.149</v>
@@ -986,17 +986,17 @@
         <v>-0.05</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.149</v>
+        <v>0.00067</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.05</v>
+        <v>0.00052</v>
       </c>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="n">
-        <v>1.01743</v>
+        <v>1.0387</v>
       </c>
       <c r="L15" t="n">
-        <v>-17.15578</v>
+        <v>-16.0046</v>
       </c>
     </row>
     <row r="16">
@@ -1007,19 +1007,19 @@
         <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>0.10944</v>
+        <v>0.09073000000000001</v>
       </c>
       <c r="D16" t="n">
-        <v>2.19456</v>
+        <v>2.32189</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.53059</v>
+        <v>-0.16993</v>
       </c>
       <c r="F16" t="n">
         <v>2.324</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.051</v>
+        <v>-0.16914</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1029,10 +1029,10 @@
       </c>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="n">
-        <v>1</v>
+        <v>1.06</v>
       </c>
       <c r="L16" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1043,32 +1043,32 @@
         <v>2</v>
       </c>
       <c r="C17" t="n">
-        <v>0.10944</v>
+        <v>0.09073000000000001</v>
       </c>
       <c r="D17" t="n">
-        <v>0.21923</v>
+        <v>0.18311</v>
       </c>
       <c r="E17" t="n">
-        <v>0.20774</v>
+        <v>0.29263</v>
       </c>
       <c r="F17" t="n">
         <v>0.183</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.08260000000000001</v>
+        <v>0.3167</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.03623</v>
+        <v>-0.00011</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
       </c>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="n">
-        <v>1</v>
+        <v>1.045</v>
       </c>
       <c r="L17" t="n">
-        <v>-5.85515</v>
+        <v>-4.98246</v>
       </c>
     </row>
     <row r="18">
@@ -1079,32 +1079,32 @@
         <v>3</v>
       </c>
       <c r="C18" t="n">
-        <v>0.10944</v>
+        <v>0.09073000000000001</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.92087</v>
+        <v>-0.94172</v>
       </c>
       <c r="E18" t="n">
-        <v>0.36428</v>
+        <v>0.05101</v>
       </c>
       <c r="F18" t="n">
         <v>-0.9419999999999999</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.0283</v>
+        <v>0.09599000000000001</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.02113</v>
+        <v>-0.00028</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
       </c>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="n">
-        <v>1</v>
+        <v>1.01</v>
       </c>
       <c r="L18" t="n">
-        <v>-14.69008</v>
+        <v>-12.72484</v>
       </c>
     </row>
     <row r="19">
@@ -1115,13 +1115,13 @@
         <v>4</v>
       </c>
       <c r="C19" t="n">
-        <v>0.10944</v>
+        <v>0.09073000000000001</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.4514</v>
+        <v>-0.47789</v>
       </c>
       <c r="E19" t="n">
-        <v>0.08903</v>
+        <v>0.03952</v>
       </c>
       <c r="F19" t="n">
         <v>-0.478</v>
@@ -1130,17 +1130,17 @@
         <v>0.039</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.0266</v>
+        <v>-0.00011</v>
       </c>
       <c r="I19" t="n">
-        <v>-0.05003</v>
+        <v>-0.00052</v>
       </c>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="n">
-        <v>0.98158</v>
+        <v>1.01768</v>
       </c>
       <c r="L19" t="n">
-        <v>-11.6924</v>
+        <v>-10.31285</v>
       </c>
     </row>
     <row r="20">
@@ -1151,13 +1151,13 @@
         <v>5</v>
       </c>
       <c r="C20" t="n">
-        <v>0.10944</v>
+        <v>0.09073000000000001</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.01914</v>
+        <v>-0.07548000000000001</v>
       </c>
       <c r="E20" t="n">
-        <v>0.09344</v>
+        <v>-0.01567</v>
       </c>
       <c r="F20" t="n">
         <v>-0.076</v>
@@ -1166,17 +1166,17 @@
         <v>-0.016</v>
       </c>
       <c r="H20" t="n">
-        <v>-0.05686</v>
+        <v>-0.00052</v>
       </c>
       <c r="I20" t="n">
-        <v>-0.10944</v>
+        <v>-0.00033</v>
       </c>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="n">
-        <v>0.9845699999999999</v>
+        <v>1.01952</v>
       </c>
       <c r="L20" t="n">
-        <v>-10.16982</v>
+        <v>-8.77369</v>
       </c>
     </row>
     <row r="21">
@@ -1187,32 +1187,32 @@
         <v>6</v>
       </c>
       <c r="C21" t="n">
-        <v>0.10944</v>
+        <v>0.09073000000000001</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.09862</v>
+        <v>-0.11183</v>
       </c>
       <c r="E21" t="n">
-        <v>0.45638</v>
+        <v>0.02895</v>
       </c>
       <c r="F21" t="n">
         <v>-0.112</v>
       </c>
       <c r="G21" t="n">
-        <v>0.35224</v>
+        <v>-0.03997</v>
       </c>
       <c r="H21" t="n">
-        <v>-0.01338</v>
+        <v>-0.00017</v>
       </c>
       <c r="I21" t="n">
-        <v>-0.10414</v>
+        <v>0</v>
       </c>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="n">
-        <v>1.08913</v>
+        <v>1.07</v>
       </c>
       <c r="L21" t="n">
-        <v>-16.3252</v>
+        <v>-14.22015</v>
       </c>
     </row>
     <row r="22">
@@ -1223,13 +1223,13 @@
         <v>7</v>
       </c>
       <c r="C22" t="n">
-        <v>0.10944</v>
+        <v>0.09073000000000001</v>
       </c>
       <c r="D22" t="n">
-        <v>0.00752</v>
+        <v>-0.00566</v>
       </c>
       <c r="E22" t="n">
-        <v>0.0102</v>
+        <v>0.09073000000000001</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -1238,17 +1238,17 @@
         <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>-0.00752</v>
+        <v>0.00566</v>
       </c>
       <c r="I22" t="n">
-        <v>-0.0102</v>
+        <v>-0.09073000000000001</v>
       </c>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="n">
-        <v>1</v>
+        <v>1.06157</v>
       </c>
       <c r="L22" t="n">
-        <v>-14.70529</v>
+        <v>-13.35962</v>
       </c>
     </row>
     <row r="23">
@@ -1259,32 +1259,32 @@
         <v>8</v>
       </c>
       <c r="C23" t="n">
-        <v>0.10944</v>
+        <v>0.09073000000000001</v>
       </c>
       <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.13274</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.55691</v>
+      </c>
+      <c r="H23" t="n">
         <v>-0</v>
       </c>
-      <c r="E23" t="n">
-        <v>-0.18425</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0</v>
-      </c>
-      <c r="G23" t="n">
-        <v>-0.19065</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0</v>
-      </c>
       <c r="I23" t="n">
-        <v>-0.0064</v>
+        <v>0</v>
       </c>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="n">
-        <v>0.97523</v>
+        <v>1.09</v>
       </c>
       <c r="L23" t="n">
-        <v>-14.70529</v>
+        <v>-13.35962</v>
       </c>
     </row>
     <row r="24">
@@ -1295,13 +1295,13 @@
         <v>9</v>
       </c>
       <c r="C24" t="n">
-        <v>0.10944</v>
+        <v>0.09073000000000001</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.29458</v>
+        <v>-0.28962</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.1549</v>
+        <v>-0.16632</v>
       </c>
       <c r="F24" t="n">
         <v>-0.295</v>
@@ -1310,17 +1310,17 @@
         <v>-0.166</v>
       </c>
       <c r="H24" t="n">
-        <v>-0.00042</v>
+        <v>-0.00538</v>
       </c>
       <c r="I24" t="n">
-        <v>-0.0111</v>
+        <v>0.00032</v>
       </c>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="n">
-        <v>1.01465</v>
+        <v>1.05596</v>
       </c>
       <c r="L24" t="n">
-        <v>-16.27269</v>
+        <v>-14.93816</v>
       </c>
     </row>
     <row r="25">
@@ -1331,13 +1331,13 @@
         <v>10</v>
       </c>
       <c r="C25" t="n">
-        <v>0.10944</v>
+        <v>0.09073000000000001</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.09279</v>
+        <v>-0.09003</v>
       </c>
       <c r="E25" t="n">
-        <v>-0.05873</v>
+        <v>-0.05784</v>
       </c>
       <c r="F25" t="n">
         <v>-0.09</v>
@@ -1346,17 +1346,17 @@
         <v>-0.058</v>
       </c>
       <c r="H25" t="n">
-        <v>0.00279</v>
+        <v>3e-05</v>
       </c>
       <c r="I25" t="n">
-        <v>0.00073</v>
+        <v>-0.00016</v>
       </c>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="n">
-        <v>1.02014</v>
+        <v>1.05101</v>
       </c>
       <c r="L25" t="n">
-        <v>-16.55157</v>
+        <v>-15.09682</v>
       </c>
     </row>
     <row r="26">
@@ -1367,13 +1367,13 @@
         <v>11</v>
       </c>
       <c r="C26" t="n">
-        <v>0.10944</v>
+        <v>0.09073000000000001</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.03836</v>
+        <v>-0.03488</v>
       </c>
       <c r="E26" t="n">
-        <v>-0.01809</v>
+        <v>-0.01782</v>
       </c>
       <c r="F26" t="n">
         <v>-0.035</v>
@@ -1382,17 +1382,17 @@
         <v>-0.018</v>
       </c>
       <c r="H26" t="n">
-        <v>0.00336</v>
+        <v>-0.00012</v>
       </c>
       <c r="I26" t="n">
-        <v>9.000000000000001e-05</v>
+        <v>-0.00018</v>
       </c>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="n">
-        <v>1.05051</v>
+        <v>1.05692</v>
       </c>
       <c r="L26" t="n">
-        <v>-16.53455</v>
+        <v>-14.78997</v>
       </c>
     </row>
     <row r="27">
@@ -1403,13 +1403,13 @@
         <v>12</v>
       </c>
       <c r="C27" t="n">
-        <v>0.10944</v>
+        <v>0.09073000000000001</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.06551</v>
+        <v>-0.06035</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.01325</v>
+        <v>-0.01477</v>
       </c>
       <c r="F27" t="n">
         <v>-0.061</v>
@@ -1418,17 +1418,17 @@
         <v>-0.016</v>
       </c>
       <c r="H27" t="n">
-        <v>0.00451</v>
+        <v>-0.00065</v>
       </c>
       <c r="I27" t="n">
-        <v>-0.00275</v>
+        <v>-0.00123</v>
       </c>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="n">
-        <v>1.07</v>
+        <v>1.05519</v>
       </c>
       <c r="L27" t="n">
-        <v>-17.14524</v>
+        <v>-15.07477</v>
       </c>
     </row>
     <row r="28">
@@ -1439,13 +1439,13 @@
         <v>13</v>
       </c>
       <c r="C28" t="n">
-        <v>0.10944</v>
+        <v>0.09073000000000001</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.13975</v>
+        <v>-0.13494</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.04613</v>
+        <v>-0.05804</v>
       </c>
       <c r="F28" t="n">
         <v>-0.135</v>
@@ -1454,17 +1454,17 @@
         <v>-0.058</v>
       </c>
       <c r="H28" t="n">
-        <v>0.00475</v>
+        <v>-6e-05</v>
       </c>
       <c r="I28" t="n">
-        <v>-0.01187</v>
+        <v>4e-05</v>
       </c>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="n">
-        <v>1.06092</v>
+        <v>1.05039</v>
       </c>
       <c r="L28" t="n">
-        <v>-17.11915</v>
+        <v>-15.15551</v>
       </c>
     </row>
     <row r="29">
@@ -1475,13 +1475,13 @@
         <v>14</v>
       </c>
       <c r="C29" t="n">
-        <v>0.10944</v>
+        <v>0.09073000000000001</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.15377</v>
+        <v>-0.149</v>
       </c>
       <c r="E29" t="n">
-        <v>-0.04841</v>
+        <v>-0.04999</v>
       </c>
       <c r="F29" t="n">
         <v>-0.149</v>
@@ -1490,17 +1490,17 @@
         <v>-0.05</v>
       </c>
       <c r="H29" t="n">
-        <v>0.00477</v>
+        <v>-0</v>
       </c>
       <c r="I29" t="n">
-        <v>-0.00159</v>
+        <v>-1e-05</v>
       </c>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="n">
-        <v>1.01648</v>
+        <v>1.03555</v>
       </c>
       <c r="L29" t="n">
-        <v>-17.67622</v>
+        <v>-16.033</v>
       </c>
     </row>
     <row r="30">
@@ -1511,19 +1511,19 @@
         <v>1</v>
       </c>
       <c r="C30" t="n">
-        <v>0.00098</v>
+        <v>0.00059</v>
       </c>
       <c r="D30" t="n">
-        <v>2.35104</v>
+        <v>2.32388</v>
       </c>
       <c r="E30" t="n">
-        <v>-0.52886</v>
+        <v>-0.16552</v>
       </c>
       <c r="F30" t="n">
         <v>2.324</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.53059</v>
+        <v>-0.16993</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
@@ -1533,10 +1533,10 @@
       </c>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="n">
-        <v>1</v>
+        <v>1.06</v>
       </c>
       <c r="L30" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1547,32 +1547,32 @@
         <v>2</v>
       </c>
       <c r="C31" t="n">
-        <v>0.00098</v>
+        <v>0.00059</v>
       </c>
       <c r="D31" t="n">
-        <v>0.18301</v>
+        <v>0.183</v>
       </c>
       <c r="E31" t="n">
-        <v>0.30997</v>
+        <v>0.30845</v>
       </c>
       <c r="F31" t="n">
         <v>0.183</v>
       </c>
       <c r="G31" t="n">
-        <v>0.20774</v>
+        <v>0.29263</v>
       </c>
       <c r="H31" t="n">
-        <v>-1e-05</v>
+        <v>-0</v>
       </c>
       <c r="I31" t="n">
         <v>0</v>
       </c>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="n">
-        <v>1</v>
+        <v>1.045</v>
       </c>
       <c r="L31" t="n">
-        <v>-5.8575</v>
+        <v>-4.98259</v>
       </c>
     </row>
     <row r="32">
@@ -1583,32 +1583,32 @@
         <v>3</v>
       </c>
       <c r="C32" t="n">
-        <v>0.00098</v>
+        <v>0.00059</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.94192</v>
+        <v>-0.94199</v>
       </c>
       <c r="E32" t="n">
-        <v>0.40487</v>
+        <v>0.06068</v>
       </c>
       <c r="F32" t="n">
         <v>-0.9419999999999999</v>
       </c>
       <c r="G32" t="n">
-        <v>0.36428</v>
+        <v>0.05101</v>
       </c>
       <c r="H32" t="n">
-        <v>-8.000000000000001e-05</v>
+        <v>-1e-05</v>
       </c>
       <c r="I32" t="n">
         <v>0</v>
       </c>
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="n">
-        <v>1</v>
+        <v>1.01</v>
       </c>
       <c r="L32" t="n">
-        <v>-14.69448</v>
+        <v>-12.7251</v>
       </c>
     </row>
     <row r="33">
@@ -1619,13 +1619,13 @@
         <v>4</v>
       </c>
       <c r="C33" t="n">
-        <v>0.00098</v>
+        <v>0.00059</v>
       </c>
       <c r="D33" t="n">
-        <v>-0.4777</v>
+        <v>-0.478</v>
       </c>
       <c r="E33" t="n">
-        <v>0.03927</v>
+        <v>0.03901</v>
       </c>
       <c r="F33" t="n">
         <v>-0.478</v>
@@ -1634,17 +1634,17 @@
         <v>0.039</v>
       </c>
       <c r="H33" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="I33" t="n">
-        <v>-0.00027</v>
+        <v>-1e-05</v>
       </c>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="n">
-        <v>0.98154</v>
+        <v>1.01767</v>
       </c>
       <c r="L33" t="n">
-        <v>-11.69663</v>
+        <v>-10.3129</v>
       </c>
     </row>
     <row r="34">
@@ -1655,13 +1655,13 @@
         <v>5</v>
       </c>
       <c r="C34" t="n">
-        <v>0.00098</v>
+        <v>0.00059</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.07562000000000001</v>
+        <v>-0.07599</v>
       </c>
       <c r="E34" t="n">
-        <v>-0.01502</v>
+        <v>-0.016</v>
       </c>
       <c r="F34" t="n">
         <v>-0.076</v>
@@ -1670,17 +1670,17 @@
         <v>-0.016</v>
       </c>
       <c r="H34" t="n">
-        <v>-0.00038</v>
+        <v>-1e-05</v>
       </c>
       <c r="I34" t="n">
-        <v>-0.00098</v>
+        <v>-0</v>
       </c>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="n">
-        <v>0.98452</v>
+        <v>1.01951</v>
       </c>
       <c r="L34" t="n">
-        <v>-10.17354</v>
+        <v>-8.773849999999999</v>
       </c>
     </row>
     <row r="35">
@@ -1691,32 +1691,32 @@
         <v>6</v>
       </c>
       <c r="C35" t="n">
-        <v>0.00098</v>
+        <v>0.00059</v>
       </c>
       <c r="D35" t="n">
-        <v>-0.11196</v>
+        <v>-0.11199</v>
       </c>
       <c r="E35" t="n">
-        <v>0.5114</v>
+        <v>0.05216</v>
       </c>
       <c r="F35" t="n">
         <v>-0.112</v>
       </c>
       <c r="G35" t="n">
-        <v>0.51136</v>
+        <v>0.02895</v>
       </c>
       <c r="H35" t="n">
-        <v>-4e-05</v>
+        <v>-1e-05</v>
       </c>
       <c r="I35" t="n">
-        <v>-4e-05</v>
+        <v>0</v>
       </c>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="n">
-        <v>1.08913</v>
+        <v>1.07</v>
       </c>
       <c r="L35" t="n">
-        <v>-16.32989</v>
+        <v>-14.22095</v>
       </c>
     </row>
     <row r="36">
@@ -1727,13 +1727,13 @@
         <v>7</v>
       </c>
       <c r="C36" t="n">
-        <v>0.00098</v>
+        <v>0.00059</v>
       </c>
       <c r="D36" t="n">
-        <v>2e-05</v>
+        <v>-6e-05</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>0.00059</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
@@ -1742,17 +1742,17 @@
         <v>0</v>
       </c>
       <c r="H36" t="n">
-        <v>-2e-05</v>
+        <v>6e-05</v>
       </c>
       <c r="I36" t="n">
-        <v>-0</v>
+        <v>-0.00059</v>
       </c>
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="n">
-        <v>1</v>
+        <v>1.06152</v>
       </c>
       <c r="L36" t="n">
-        <v>-14.70983</v>
+        <v>-13.35963</v>
       </c>
     </row>
     <row r="37">
@@ -1763,32 +1763,32 @@
         <v>8</v>
       </c>
       <c r="C37" t="n">
-        <v>0.00098</v>
+        <v>0.00059</v>
       </c>
       <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.17595</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.13274</v>
+      </c>
+      <c r="H37" t="n">
         <v>-0</v>
       </c>
-      <c r="E37" t="n">
-        <v>-0.13713</v>
-      </c>
-      <c r="F37" t="n">
-        <v>0</v>
-      </c>
-      <c r="G37" t="n">
-        <v>-0.13757</v>
-      </c>
-      <c r="H37" t="n">
-        <v>0</v>
-      </c>
       <c r="I37" t="n">
-        <v>-0.00044</v>
+        <v>0</v>
       </c>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="n">
-        <v>0.97528</v>
+        <v>1.09</v>
       </c>
       <c r="L37" t="n">
-        <v>-14.70983</v>
+        <v>-13.35963</v>
       </c>
     </row>
     <row r="38">
@@ -1799,13 +1799,13 @@
         <v>9</v>
       </c>
       <c r="C38" t="n">
-        <v>0.00098</v>
+        <v>0.00059</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.295</v>
+        <v>-0.29495</v>
       </c>
       <c r="E38" t="n">
-        <v>-0.16598</v>
+        <v>-0.16599</v>
       </c>
       <c r="F38" t="n">
         <v>-0.295</v>
@@ -1814,17 +1814,17 @@
         <v>-0.166</v>
       </c>
       <c r="H38" t="n">
-        <v>-0</v>
+        <v>-5e-05</v>
       </c>
       <c r="I38" t="n">
-        <v>-2e-05</v>
+        <v>-1e-05</v>
       </c>
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="n">
-        <v>1.01464</v>
+        <v>1.05593</v>
       </c>
       <c r="L38" t="n">
-        <v>-16.2772</v>
+        <v>-14.93852</v>
       </c>
     </row>
     <row r="39">
@@ -1835,10 +1835,10 @@
         <v>10</v>
       </c>
       <c r="C39" t="n">
-        <v>0.00098</v>
+        <v>0.00059</v>
       </c>
       <c r="D39" t="n">
-        <v>-0.09001000000000001</v>
+        <v>-0.08999</v>
       </c>
       <c r="E39" t="n">
         <v>-0.058</v>
@@ -1850,17 +1850,17 @@
         <v>-0.058</v>
       </c>
       <c r="H39" t="n">
-        <v>1e-05</v>
+        <v>-1e-05</v>
       </c>
       <c r="I39" t="n">
         <v>-0</v>
       </c>
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="n">
-        <v>1.02013</v>
+        <v>1.05098</v>
       </c>
       <c r="L39" t="n">
-        <v>-16.5561</v>
+        <v>-15.09729</v>
       </c>
     </row>
     <row r="40">
@@ -1871,10 +1871,10 @@
         <v>11</v>
       </c>
       <c r="C40" t="n">
-        <v>0.00098</v>
+        <v>0.00059</v>
       </c>
       <c r="D40" t="n">
-        <v>-0.035</v>
+        <v>-0.03499</v>
       </c>
       <c r="E40" t="n">
         <v>-0.018</v>
@@ -1886,17 +1886,17 @@
         <v>-0.018</v>
       </c>
       <c r="H40" t="n">
-        <v>-0</v>
+        <v>-1e-05</v>
       </c>
       <c r="I40" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="n">
-        <v>1.05051</v>
+        <v>1.05691</v>
       </c>
       <c r="L40" t="n">
-        <v>-16.53917</v>
+        <v>-14.79062</v>
       </c>
     </row>
     <row r="41">
@@ -1907,7 +1907,7 @@
         <v>12</v>
       </c>
       <c r="C41" t="n">
-        <v>0.00098</v>
+        <v>0.00059</v>
       </c>
       <c r="D41" t="n">
         <v>-0.061</v>
@@ -1929,10 +1929,10 @@
       </c>
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="n">
-        <v>1.07</v>
+        <v>1.05519</v>
       </c>
       <c r="L41" t="n">
-        <v>-17.14995</v>
+        <v>-15.07558</v>
       </c>
     </row>
     <row r="42">
@@ -1943,13 +1943,13 @@
         <v>13</v>
       </c>
       <c r="C42" t="n">
-        <v>0.00098</v>
+        <v>0.00059</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.13499</v>
+        <v>-0.135</v>
       </c>
       <c r="E42" t="n">
-        <v>-0.05799</v>
+        <v>-0.058</v>
       </c>
       <c r="F42" t="n">
         <v>-0.135</v>
@@ -1958,17 +1958,17 @@
         <v>-0.058</v>
       </c>
       <c r="H42" t="n">
-        <v>-1e-05</v>
+        <v>-0</v>
       </c>
       <c r="I42" t="n">
-        <v>-1e-05</v>
+        <v>0</v>
       </c>
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="n">
-        <v>1.06092</v>
+        <v>1.05038</v>
       </c>
       <c r="L42" t="n">
-        <v>-17.12381</v>
+        <v>-15.15628</v>
       </c>
     </row>
     <row r="43">
@@ -1979,13 +1979,13 @@
         <v>14</v>
       </c>
       <c r="C43" t="n">
-        <v>0.00098</v>
+        <v>0.00059</v>
       </c>
       <c r="D43" t="n">
-        <v>-0.14901</v>
+        <v>-0.14899</v>
       </c>
       <c r="E43" t="n">
-        <v>-0.04999</v>
+        <v>-0.05</v>
       </c>
       <c r="F43" t="n">
         <v>-0.149</v>
@@ -1994,17 +1994,17 @@
         <v>-0.05</v>
       </c>
       <c r="H43" t="n">
-        <v>1e-05</v>
+        <v>-1e-05</v>
       </c>
       <c r="I43" t="n">
-        <v>-1e-05</v>
+        <v>0</v>
       </c>
       <c r="J43" t="inlineStr"/>
       <c r="K43" t="n">
-        <v>1.01647</v>
+        <v>1.03553</v>
       </c>
       <c r="L43" t="n">
-        <v>-17.68071</v>
+        <v>-16.03364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>